<commit_message>
Fixed missing image for Victor 2
</commit_message>
<xml_diff>
--- a/data/cards.xlsx
+++ b/data/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shipcards\shipcards\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FED9BF7-E419-43CA-A84D-C2BCA824F0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DFE5BD-B606-4779-9A72-7A9A66E5589E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="7500" windowHeight="6000" xr2:uid="{F50BFA29-F894-47F8-8978-4D4DA77633D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{F50BFA29-F894-47F8-8978-4D4DA77633D4}"/>
   </bookViews>
   <sheets>
     <sheet name="military_asset_final" sheetId="7" r:id="rId1"/>
@@ -22,11 +22,6 @@
     <sheet name="territories" sheetId="5" r:id="rId7"/>
     <sheet name="balance" sheetId="6" r:id="rId8"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">balance!$N$29:$N$54</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">balance!$O$28</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">balance!$O$29:$O$54</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -67,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="286">
   <si>
     <t>Title</t>
   </si>
@@ -922,6 +917,9 @@
   </si>
   <si>
     <t>Volk</t>
+  </si>
+  <si>
+    <t>Images/victor2.jpg</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1103,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15083298-1658-4A69-B28D-243BD43CB66C}" type="CELLRANGE">
+                    <a:fld id="{21B95892-6DA9-4034-953E-47FD8B47E898}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1139,7 +1137,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A32BECBF-866A-4C0C-B583-EB7902D24E19}" type="CELLRANGE">
+                    <a:fld id="{A4231283-7E2E-4DC7-AE2B-44E04DC1142A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1173,7 +1171,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34EF18BD-1764-4B79-9B3B-FBCD33AD7FF9}" type="CELLRANGE">
+                    <a:fld id="{E9F0132E-E280-4B85-8EF4-FF321211C5F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1213,7 +1211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC02E098-4D3B-40E2-8942-360E7C0D2F77}" type="CELLRANGE">
+                    <a:fld id="{57D3DD51-218C-40F4-9E95-A2D1B5B203AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1252,7 +1250,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2FCD011-1021-4B19-8CD0-89901BFF803F}" type="CELLRANGE">
+                    <a:fld id="{B9E08673-4B86-4A40-B222-A79D92C40D26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1285,7 +1283,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0787FDBD-D43D-4E8C-9F27-93C7FC830F4B}" type="CELLRANGE">
+                    <a:fld id="{D66BC644-C4DC-415A-82CC-2FEA5E75CC4F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1319,7 +1317,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCFFF8FB-4A0F-4C2D-AC15-3D928EB23DDF}" type="CELLRANGE">
+                    <a:fld id="{50910983-ED6D-467C-93DC-F1B555E1E704}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1359,7 +1357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3ADB6F29-0F85-4C92-B2AF-067A66B46776}" type="CELLRANGE">
+                    <a:fld id="{AA8CA188-EE14-46F9-B68D-859462EDC83D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1398,7 +1396,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60699A83-485E-46A2-B1AC-D9F33BEA2CA6}" type="CELLRANGE">
+                    <a:fld id="{CB276A3A-3054-450A-AED0-3AA6803D190A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1431,7 +1429,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5CA9E40-0FE5-4B11-9CA2-F39B04CF4D9E}" type="CELLRANGE">
+                    <a:fld id="{C954CC9B-38F2-4117-AA4C-30113B8E4B70}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1471,7 +1469,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63D62B9A-0835-47D2-A360-7DF686C0ADC8}" type="CELLRANGE">
+                    <a:fld id="{97B32F66-96EB-4510-901E-3097ADC08E26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1525,7 +1523,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{AAAA77CF-34DC-4D7A-98BA-6FCE5C2CFDF2}" type="CELLRANGE">
+                    <a:fld id="{79918D58-3D55-4D99-895A-E0F09CA24296}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -1595,7 +1593,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B2614AB-2838-4F2E-8672-2F7C3A3F37AD}" type="CELLRANGE">
+                    <a:fld id="{FB044824-FED1-455D-9CF7-7D4FBE9085DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1635,7 +1633,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ADA0CF31-4BA6-4E2D-96FF-167CC50A51C4}" type="CELLRANGE">
+                    <a:fld id="{5AE982CD-46EF-41E9-9408-B07203E3A14E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1674,7 +1672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38E4270B-EADB-40FF-A460-726DBFE986B1}" type="CELLRANGE">
+                    <a:fld id="{A2EB8403-6DDE-432A-BC5A-1CEA46F2F5FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1707,7 +1705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A65ECFC2-6312-4F14-A3B5-D7B186D0B363}" type="CELLRANGE">
+                    <a:fld id="{79EA1A9A-F745-41B9-9AD1-1115D220C81A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1747,7 +1745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41737ADB-53F9-4F3D-A3FF-C9964E367E53}" type="CELLRANGE">
+                    <a:fld id="{A6F46525-8462-428D-9E12-E6DE4324CB99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1801,7 +1799,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{A9C7796C-6689-4AB2-9FFF-28BFA6159E83}" type="CELLRANGE">
+                    <a:fld id="{98C82D7E-F71F-47BB-B3C7-96C9D1838DB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -1877,7 +1875,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{060F4797-7685-4066-B4AE-CDD5E1841CDB}" type="CELLRANGE">
+                    <a:fld id="{0D4DEA62-63D2-4008-81FB-DA3E03E3D069}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1916,7 +1914,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4F4509D-3DCB-420C-A905-B1FC2CB8D9D7}" type="CELLRANGE">
+                    <a:fld id="{57A26F14-7606-4BBC-AAF6-6C4A5070F0D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1955,7 +1953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96751F0D-A27D-4F35-8973-80D0588E728B}" type="CELLRANGE">
+                    <a:fld id="{ED2CC525-4108-4D4C-9F2A-4368CA083E02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1994,7 +1992,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{524DA7CD-3C10-4C6C-A8FA-AB0A9CA8AEEF}" type="CELLRANGE">
+                    <a:fld id="{C33EB8AE-80C4-4898-8E6A-7DD1FBDFCFFD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2027,7 +2025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8045BFE9-3E27-48CE-A3D9-B907B7BFF4C9}" type="CELLRANGE">
+                    <a:fld id="{2FCED977-1C94-4180-AFB6-C4D65CD2FAD4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2067,7 +2065,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35C15702-AD20-4E1C-8DC0-0608FBA25E0A}" type="CELLRANGE">
+                    <a:fld id="{15088E43-A2C7-4B9D-B385-5B3312FB241C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2100,7 +2098,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96035AFD-2092-41F7-B9CA-93D4EC24FF17}" type="CELLRANGE">
+                    <a:fld id="{C4CFEE3B-221E-4BC2-B895-4D7105E70182}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2140,7 +2138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C53CD4B4-16E5-431B-A56F-0AF034B01460}" type="CELLRANGE">
+                    <a:fld id="{972D6428-29EB-46BF-8035-08E1C11414DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3604,7 +3602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E8987D-349F-4742-AF8A-4428C54D0A0B}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -6283,9 +6281,9 @@
 Ambush: This asset deals damage during the Ambush Damage Step.
 Commerce Raider: When assaulting a player, this military asset's assault is equal to its attack.</v>
       </c>
-      <c r="O39" cm="1">
+      <c r="O39" t="str" cm="1">
         <f t="array" aca="1" ref="O39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
-        <v>0</v>
+        <v>Images/victor2.jpg</v>
       </c>
       <c r="P39" t="str" cm="1">
         <f t="array" aca="1" ref="P39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
@@ -6352,9 +6350,9 @@
 Ambush: This asset deals damage during the Ambush Damage Step.
 Commerce Raider: When assaulting a player, this military asset's assault is equal to its attack.</v>
       </c>
-      <c r="O40" cm="1">
+      <c r="O40" t="str" cm="1">
         <f t="array" aca="1" ref="O40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
-        <v>0</v>
+        <v>Images/victor2.jpg</v>
       </c>
       <c r="P40" t="str" cm="1">
         <f t="array" aca="1" ref="P40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
@@ -6582,9 +6580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA93C54-FC77-4A57-AEDF-D4D1B82432EF}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7584,6 +7582,9 @@
         <v>Hidden: Can be played face down. 
 Ambush: This asset deals damage during the Ambush Damage Step.
 Commerce Raider: When assaulting a player, this military asset's assault is equal to its attack.</v>
+      </c>
+      <c r="L26" t="s">
+        <v>285</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>275</v>

</xml_diff>

<commit_message>
Issue #23: Fix version system
</commit_message>
<xml_diff>
--- a/data/cards.xlsx
+++ b/data/cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shipcards\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEADDAD7-6836-4A3D-9299-94278AFA5597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC657CD-E64A-44FF-8CA6-D69363AD4F4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="771" firstSheet="3" activeTab="3" xr2:uid="{F50BFA29-F894-47F8-8978-4D4DA77633D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="771" firstSheet="3" activeTab="7" xr2:uid="{F50BFA29-F894-47F8-8978-4D4DA77633D4}"/>
   </bookViews>
   <sheets>
     <sheet name="military_asset_final" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <sheet name="balance" sheetId="6" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="326">
   <si>
     <t>Title</t>
   </si>
@@ -1045,6 +1044,9 @@
   </si>
   <si>
     <t>Retrieve one card from your discard pile, reveal it, and put it on top of your deck.</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1230,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFE3DCB4-DECA-4F91-8FD2-915575922F6F}" type="CELLRANGE">
+                    <a:fld id="{19BA67ED-4F2F-41CA-87A3-6166B158FDCE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1262,7 +1264,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{391D0FF1-51D3-473B-9BB7-6FB00E95D66F}" type="CELLRANGE">
+                    <a:fld id="{5E2B0500-1483-48A2-9DB7-2D2D99917D39}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1296,7 +1298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE006581-1DB7-4C9B-A3B7-38A8F66168BA}" type="CELLRANGE">
+                    <a:fld id="{E74652AB-D54D-41E7-806F-819658DEF1A0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1336,7 +1338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB44B4EE-A735-4D13-BBB1-C4D76FD2C5BF}" type="CELLRANGE">
+                    <a:fld id="{39894B46-29A0-4FC2-A910-27540CFA4590}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1375,7 +1377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48B472A8-579E-45F3-BACF-020CB5108DCF}" type="CELLRANGE">
+                    <a:fld id="{83A3DE41-B9ED-43B0-AF1B-E41308D6D5B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1408,7 +1410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4B65C53-8B65-40EF-9D51-412144CB9C06}" type="CELLRANGE">
+                    <a:fld id="{0F53F70E-912F-49E8-AED7-B1D1EA67BCA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1442,7 +1444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3800F9D2-470A-4A31-B63B-1B13D54703C8}" type="CELLRANGE">
+                    <a:fld id="{9019098A-83AE-4542-B790-4355FA624914}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1482,7 +1484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{087C0AF0-B135-493B-A7C9-C0229ED3DF52}" type="CELLRANGE">
+                    <a:fld id="{616FC26D-5A7D-4B09-B80A-AE45A4B1BD76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1521,7 +1523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F0716B3-2784-4E05-B4C2-D487AA1E054D}" type="CELLRANGE">
+                    <a:fld id="{07F33445-D379-4262-A89F-CF041F6D3D08}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1554,7 +1556,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{704AA7F6-2782-4F5F-9F23-CB2CFF3F88AF}" type="CELLRANGE">
+                    <a:fld id="{FA4398A4-CCDA-4103-8ED9-0331E9D4A557}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1594,7 +1596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C29CAE3B-30E7-4264-8465-0951E82D009F}" type="CELLRANGE">
+                    <a:fld id="{1F8E7AF0-3961-4275-BCD6-C0D6C2B378E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1648,7 +1650,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{6011BA4C-8972-4C79-98BA-044701789BBA}" type="CELLRANGE">
+                    <a:fld id="{9E34D7E7-A15C-4811-9CD2-230BAC99A0E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -1718,7 +1720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39D1835E-F063-4B3D-8BEF-677EABB6D1FC}" type="CELLRANGE">
+                    <a:fld id="{F0AB681F-341E-4FFA-ADCB-29964A00581A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1758,7 +1760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A69858E7-4101-40B1-BCAA-F2C0899EE21B}" type="CELLRANGE">
+                    <a:fld id="{3DBAFC33-3F8F-4579-B0E3-60E1ECA3B0BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1797,7 +1799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A31B30B-332D-4480-B91C-A2E766AEE543}" type="CELLRANGE">
+                    <a:fld id="{0FCAD41C-10FD-441B-B5B1-EB8FE1EC9E46}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1830,7 +1832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA38E466-2E49-4CB7-B34C-9C6BFFEEE53A}" type="CELLRANGE">
+                    <a:fld id="{67DE8F01-B11E-45C3-BC67-DFA7E805815B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1870,7 +1872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0B56A14-4C04-4FF9-ACCA-66E8E86FF6F1}" type="CELLRANGE">
+                    <a:fld id="{DD823903-9C45-42B9-AD32-D2E4ECC135EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1924,7 +1926,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{72AE5106-B55B-4312-83D0-A1613064DC0A}" type="CELLRANGE">
+                    <a:fld id="{E161E9DB-9B33-44F7-B8A4-C1FF4535152A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -2000,7 +2002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14579CD3-6E47-4DC8-85C1-6BED864C64D1}" type="CELLRANGE">
+                    <a:fld id="{7903D458-807C-46A6-A6AB-2BFBBD70CCF1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2039,7 +2041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0019778D-9663-433F-8C25-D3AF5C6EF234}" type="CELLRANGE">
+                    <a:fld id="{8180A7E4-2060-4688-B47C-A3A48CF709EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2078,7 +2080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C9207A6-B3C3-4844-906A-3BF7563F28D7}" type="CELLRANGE">
+                    <a:fld id="{81CC247B-EB05-43F1-8C11-F61E30A93409}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2117,7 +2119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40591A13-B07E-4A96-ABEC-E7CB61CC7984}" type="CELLRANGE">
+                    <a:fld id="{0AD1A498-FB87-498E-B3D3-336B3BB56FE1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2150,7 +2152,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C6DA128-EDC3-42E8-A526-7DD7B5B46FE4}" type="CELLRANGE">
+                    <a:fld id="{C5CE632A-64D5-4D8C-A9A1-BA101A9EEF7B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2190,7 +2192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E1DC391-D79D-48EE-B100-F612E2810046}" type="CELLRANGE">
+                    <a:fld id="{BFE0FD21-7B8C-4EBB-ADB4-D9C88F859919}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2223,7 +2225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F43F23D-7E2E-4122-B956-292B189F1E4E}" type="CELLRANGE">
+                    <a:fld id="{11D789D7-720A-48DA-901D-136427CE4D93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2263,7 +2265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E71D7770-B90A-4743-A5F8-50CF170C8C97}" type="CELLRANGE">
+                    <a:fld id="{4AD3F2A5-1B94-4325-964F-94BDF7AAF084}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2296,7 +2298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{150F4CEA-EEB7-4935-BE6D-35C2F6437131}" type="CELLRANGE">
+                    <a:fld id="{298D96FA-95B3-4FFE-8FB8-8A5FF872DCB5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3935,9 +3937,9 @@
         <f t="array" aca="1" ref="P2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>A military airbase at sea, a Nimitz carrier is more than three times as long as a football field and has more than twice the displacement of the German super-battleship Bismarck.</v>
       </c>
-      <c r="Q2" cm="1">
+      <c r="Q2" t="str" cm="1">
         <f t="array" aca="1" ref="Q2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -4004,9 +4006,9 @@
         <f t="array" aca="1" ref="P3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>A military airbase at sea, a Nimitz carrier is more than three times as long as a football field and has more than twice the displacement of the German super-battleship Bismarck.</v>
       </c>
-      <c r="Q3" cm="1">
+      <c r="Q3" t="str" cm="1">
         <f t="array" aca="1" ref="Q3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -4073,9 +4075,9 @@
         <f t="array" aca="1" ref="P4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>A military airbase at sea, a Nimitz carrier is more than three times as long as a football field and has more than twice the displacement of the German super-battleship Bismarck.</v>
       </c>
-      <c r="Q4" cm="1">
+      <c r="Q4" t="str" cm="1">
         <f t="array" aca="1" ref="Q4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -4141,9 +4143,9 @@
         <f t="array" aca="1" ref="P5" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q5" cm="1">
+      <c r="Q5" t="str" cm="1">
         <f t="array" aca="1" ref="Q5" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -4209,9 +4211,9 @@
         <f t="array" aca="1" ref="P6" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q6" cm="1">
+      <c r="Q6" t="str" cm="1">
         <f t="array" aca="1" ref="Q6" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -4277,9 +4279,9 @@
         <f t="array" aca="1" ref="P7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q7" cm="1">
+      <c r="Q7" t="str" cm="1">
         <f t="array" aca="1" ref="Q7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -4345,9 +4347,9 @@
         <f t="array" aca="1" ref="P8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q8" cm="1">
+      <c r="Q8" t="str" cm="1">
         <f t="array" aca="1" ref="Q8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4413,9 +4415,9 @@
         <f t="array" aca="1" ref="P9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q9" cm="1">
+      <c r="Q9" t="str" cm="1">
         <f t="array" aca="1" ref="Q9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -4483,9 +4485,9 @@
         <f t="array" aca="1" ref="P10" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
         <v>As the most expensive class of attack submarine ever built, the Seawolf is the apex predator of the US Navy's submarine fleet.</v>
       </c>
-      <c r="Q10" cm="1">
+      <c r="Q10" t="str" cm="1">
         <f t="array" aca="1" ref="Q10" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -4552,9 +4554,9 @@
         <f t="array" aca="1" ref="P11" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
         <v>The advanced Virginia will be the standard attack submarine of the US Navy until at least the middle of the 21st century.</v>
       </c>
-      <c r="Q11" cm="1">
+      <c r="Q11" t="str" cm="1">
         <f t="array" aca="1" ref="Q11" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4621,9 +4623,9 @@
         <f t="array" aca="1" ref="P12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
         <v>The advanced Virginia will be the standard attack submarine of the US Navy until at least the middle of the 21st century.</v>
       </c>
-      <c r="Q12" cm="1">
+      <c r="Q12" t="str" cm="1">
         <f t="array" aca="1" ref="Q12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4690,9 +4692,9 @@
         <f t="array" aca="1" ref="P13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
         <v>The advanced Virginia will be the standard attack submarine of the US Navy until at least the middle of the 21st century.</v>
       </c>
-      <c r="Q13" cm="1">
+      <c r="Q13" t="str" cm="1">
         <f t="array" aca="1" ref="Q13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -4759,9 +4761,9 @@
         <f t="array" aca="1" ref="P14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
         <v>Although Ohio was originally intended to carry nuclear ballistic missiles, some Ohio's have been modified as SSGNs for surface warfare and land-attack missions.</v>
       </c>
-      <c r="Q14" cm="1">
+      <c r="Q14" t="str" cm="1">
         <f t="array" aca="1" ref="Q14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -4828,9 +4830,9 @@
         <f t="array" aca="1" ref="P15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
         <v>Although Ohio was originally intended to carry nuclear ballistic missiles, some Ohio's have been modified as SSGNs for surface warfare and land-attack missions.</v>
       </c>
-      <c r="Q15" cm="1">
+      <c r="Q15" t="str" cm="1">
         <f t="array" aca="1" ref="Q15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -4895,9 +4897,9 @@
         <f t="array" aca="1" ref="P16" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
         <v>Despite a modest displacement by historical standards, the Ticonderoga is the largest surface combatant in the US Navy.</v>
       </c>
-      <c r="Q16" cm="1">
+      <c r="Q16" t="str" cm="1">
         <f t="array" aca="1" ref="Q16" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -4962,9 +4964,9 @@
         <f t="array" aca="1" ref="P17" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
         <v>Despite a modest displacement by historical standards, the Ticonderoga is the largest surface combatant in the US Navy.</v>
       </c>
-      <c r="Q17" cm="1">
+      <c r="Q17" t="str" cm="1">
         <f t="array" aca="1" ref="Q17" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -5029,9 +5031,9 @@
         <f t="array" aca="1" ref="P18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
         <v>Despite a modest displacement by historical standards, the Ticonderoga is the largest surface combatant in the US Navy.</v>
       </c>
-      <c r="Q18" cm="1">
+      <c r="Q18" t="str" cm="1">
         <f t="array" aca="1" ref="Q18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -5096,9 +5098,9 @@
         <f t="array" aca="1" ref="P19" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q19" cm="1">
+      <c r="Q19" t="str" cm="1">
         <f t="array" aca="1" ref="Q19" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -5163,9 +5165,9 @@
         <f t="array" aca="1" ref="P20" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q20" cm="1">
+      <c r="Q20" t="str" cm="1">
         <f t="array" aca="1" ref="Q20" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -5230,9 +5232,9 @@
         <f t="array" aca="1" ref="P21" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q21" cm="1">
+      <c r="Q21" t="str" cm="1">
         <f t="array" aca="1" ref="Q21" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -5297,9 +5299,9 @@
         <f t="array" aca="1" ref="P22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q22" cm="1">
+      <c r="Q22" t="str" cm="1">
         <f t="array" aca="1" ref="Q22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -5364,9 +5366,9 @@
         <f t="array" aca="1" ref="P23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q23" cm="1">
+      <c r="Q23" t="str" cm="1">
         <f t="array" aca="1" ref="Q23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -5431,9 +5433,9 @@
         <f t="array" aca="1" ref="P24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
         <v>With a cost of $1M per shot from its main howitzer, it is important for the crew of a Zumwalt to aim carefully.</v>
       </c>
-      <c r="Q24" cm="1">
+      <c r="Q24" t="str" cm="1">
         <f t="array" aca="1" ref="Q24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -5498,9 +5500,9 @@
         <f t="array" aca="1" ref="P25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
         <v>With a cost of $1M per shot from its main howitzer, it is important for the crew of a Zumwalt to aim carefully.</v>
       </c>
-      <c r="Q25" cm="1">
+      <c r="Q25" t="str" cm="1">
         <f t="array" aca="1" ref="Q25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -5566,9 +5568,9 @@
         <f t="array" aca="1" ref="P26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q26" cm="1">
+      <c r="Q26" t="str" cm="1">
         <f t="array" aca="1" ref="Q26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -5634,9 +5636,9 @@
         <f t="array" aca="1" ref="P27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q27" cm="1">
+      <c r="Q27" t="str" cm="1">
         <f t="array" aca="1" ref="Q27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -5702,9 +5704,9 @@
         <f t="array" aca="1" ref="P28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q28" cm="1">
+      <c r="Q28" t="str" cm="1">
         <f t="array" aca="1" ref="Q28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -5770,9 +5772,9 @@
         <f t="array" aca="1" ref="P29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q29" cm="1">
+      <c r="Q29" t="str" cm="1">
         <f t="array" aca="1" ref="Q29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -5838,9 +5840,9 @@
         <f t="array" aca="1" ref="P30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q30" cm="1">
+      <c r="Q30" t="str" cm="1">
         <f t="array" aca="1" ref="Q30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -5907,9 +5909,9 @@
         <f t="array" aca="1" ref="P31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
         <v>The F-35B is a special variant of the F-35 capable of taking off and landing vertically. This allows it to be stationed on smaller carriers that have typically not been able to field cutting-edge aircraft.</v>
       </c>
-      <c r="Q31" cm="1">
+      <c r="Q31" t="str" cm="1">
         <f t="array" aca="1" ref="Q31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -5976,9 +5978,9 @@
         <f t="array" aca="1" ref="P32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
         <v>The F-35B is a special variant of the F-35 capable of taking off and landing vertically. This allows it to be stationed on smaller carriers that have typically not been able to field cutting-edge aircraft.</v>
       </c>
-      <c r="Q32" cm="1">
+      <c r="Q32" t="str" cm="1">
         <f t="array" aca="1" ref="Q32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -6045,9 +6047,9 @@
         <f t="array" aca="1" ref="P33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
         <v>The F-35B is a special variant of the F-35 capable of taking off and landing vertically. This allows it to be stationed on smaller carriers that have typically not been able to field cutting-edge aircraft.</v>
       </c>
-      <c r="Q33" cm="1">
+      <c r="Q33" t="str" cm="1">
         <f t="array" aca="1" ref="Q33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -6114,9 +6116,9 @@
         <f t="array" aca="1" ref="P34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
         <v>The F-35 acquisition program cost of just under $450 billion USD would be enough to buy 450 billion $1 cheeseburgers - enough to kill all humans on earth.</v>
       </c>
-      <c r="Q34" cm="1">
+      <c r="Q34" t="str" cm="1">
         <f t="array" aca="1" ref="Q34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -6183,9 +6185,9 @@
         <f t="array" aca="1" ref="P35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
         <v>The F-35 acquisition program cost of just under $450 billion USD would be enough to buy 450 billion $1 cheeseburgers - enough to kill all humans on earth.</v>
       </c>
-      <c r="Q35" cm="1">
+      <c r="Q35" t="str" cm="1">
         <f t="array" aca="1" ref="Q35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -6252,9 +6254,9 @@
         <f t="array" aca="1" ref="P36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
         <v>The F-35 acquisition program cost of just under $450 billion USD would be enough to buy 450 billion $1 cheeseburgers - enough to kill all humans on earth.</v>
       </c>
-      <c r="Q36" cm="1">
+      <c r="Q36" t="str" cm="1">
         <f t="array" aca="1" ref="Q36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -6320,9 +6322,9 @@
         <f t="array" aca="1" ref="P37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q37" cm="1">
+      <c r="Q37" t="str" cm="1">
         <f t="array" aca="1" ref="Q37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -6388,9 +6390,9 @@
         <f t="array" aca="1" ref="P38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q38" cm="1">
+      <c r="Q38" t="str" cm="1">
         <f t="array" aca="1" ref="Q38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -6456,9 +6458,9 @@
         <f t="array" aca="1" ref="P39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q39" cm="1">
+      <c r="Q39" t="str" cm="1">
         <f t="array" aca="1" ref="Q39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -6524,9 +6526,9 @@
         <f t="array" aca="1" ref="P40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q40" cm="1">
+      <c r="Q40" t="str" cm="1">
         <f t="array" aca="1" ref="Q40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -6592,9 +6594,9 @@
         <f t="array" aca="1" ref="P41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q41" cm="1">
+      <c r="Q41" t="str" cm="1">
         <f t="array" aca="1" ref="Q41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -6660,9 +6662,9 @@
         <f t="array" aca="1" ref="P42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
         <v>Although sold to a company in Macau supposedly for use as a floating casino, Kuznetsov's sister ship has since unsurprisingly become the first aircraft carrier of the Chinese People's Liberation Army Navy.</v>
       </c>
-      <c r="Q42" cm="1">
+      <c r="Q42" t="str" cm="1">
         <f t="array" aca="1" ref="Q42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -6727,9 +6729,9 @@
         <f t="array" aca="1" ref="P43" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B43)</f>
         <v>Since the decommisioning of the last retrofitted WWII-era battleship in 1991, the Kirov has been the largest surface combatant in the world.</v>
       </c>
-      <c r="Q43" cm="1">
+      <c r="Q43" t="str" cm="1">
         <f t="array" aca="1" ref="Q43" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B43)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -6794,9 +6796,9 @@
         <f t="array" aca="1" ref="P44" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B44)</f>
         <v>Since the decommisioning of the last retrofitted WWII-era battleship in 1991, the Kirov has been the largest surface combatant in the world.</v>
       </c>
-      <c r="Q44" cm="1">
+      <c r="Q44" t="str" cm="1">
         <f t="array" aca="1" ref="Q44" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B44)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -6861,9 +6863,9 @@
         <f t="array" aca="1" ref="P45" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B45)</f>
         <v>Since the decommisioning of the last retrofitted WWII-era battleship in 1991, the Kirov has been the largest surface combatant in the world.</v>
       </c>
-      <c r="Q45" cm="1">
+      <c r="Q45" t="str" cm="1">
         <f t="array" aca="1" ref="Q45" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B45)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -6928,9 +6930,9 @@
         <f t="array" aca="1" ref="P46" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B46)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q46" cm="1">
+      <c r="Q46" t="str" cm="1">
         <f t="array" aca="1" ref="Q46" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B46)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -6995,9 +6997,9 @@
         <f t="array" aca="1" ref="P47" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B47)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q47" cm="1">
+      <c r="Q47" t="str" cm="1">
         <f t="array" aca="1" ref="Q47" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B47)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -7062,9 +7064,9 @@
         <f t="array" aca="1" ref="P48" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B48)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q48" cm="1">
+      <c r="Q48" t="str" cm="1">
         <f t="array" aca="1" ref="Q48" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B48)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -7129,9 +7131,9 @@
         <f t="array" aca="1" ref="P49" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B49)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q49" cm="1">
+      <c r="Q49" t="str" cm="1">
         <f t="array" aca="1" ref="Q49" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B49)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -7197,9 +7199,9 @@
         <f t="array" aca="1" ref="P50" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B50)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q50" cm="1">
+      <c r="Q50" t="str" cm="1">
         <f t="array" aca="1" ref="Q50" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B50)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -7265,9 +7267,9 @@
         <f t="array" aca="1" ref="P51" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B51)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q51" cm="1">
+      <c r="Q51" t="str" cm="1">
         <f t="array" aca="1" ref="Q51" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B51)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -7333,9 +7335,9 @@
         <f t="array" aca="1" ref="P52" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B52)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q52" cm="1">
+      <c r="Q52" t="str" cm="1">
         <f t="array" aca="1" ref="Q52" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B52)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -7401,9 +7403,9 @@
         <f t="array" aca="1" ref="P53" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B53)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q53" cm="1">
+      <c r="Q53" t="str" cm="1">
         <f t="array" aca="1" ref="Q53" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B53)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -7469,9 +7471,9 @@
         <f t="array" aca="1" ref="P54" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B54)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q54" cm="1">
+      <c r="Q54" t="str" cm="1">
         <f t="array" aca="1" ref="Q54" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B54)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -7537,9 +7539,9 @@
         <f t="array" aca="1" ref="P55" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B55)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q55" cm="1">
+      <c r="Q55" t="str" cm="1">
         <f t="array" aca="1" ref="Q55" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B55)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -7605,9 +7607,9 @@
         <f t="array" aca="1" ref="P56" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B56)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q56" cm="1">
+      <c r="Q56" t="str" cm="1">
         <f t="array" aca="1" ref="Q56" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B56)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -7673,9 +7675,9 @@
         <f t="array" aca="1" ref="P57" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B57)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q57" cm="1">
+      <c r="Q57" t="str" cm="1">
         <f t="array" aca="1" ref="Q57" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B57)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -7741,9 +7743,9 @@
         <f t="array" aca="1" ref="P58" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B58)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q58" cm="1">
+      <c r="Q58" t="str" cm="1">
         <f t="array" aca="1" ref="Q58" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B58)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -7809,9 +7811,9 @@
         <f t="array" aca="1" ref="P59" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B59)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q59" cm="1">
+      <c r="Q59" t="str" cm="1">
         <f t="array" aca="1" ref="Q59" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B59)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -7876,9 +7878,9 @@
         <f t="array" aca="1" ref="P60" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B60)</f>
         <v>The cutting-edge Gorshkov frigates stick out in the largely-outdated Russian surface warfare fleet.</v>
       </c>
-      <c r="Q60" cm="1">
+      <c r="Q60" t="str" cm="1">
         <f t="array" aca="1" ref="Q60" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B60)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -7943,9 +7945,9 @@
         <f t="array" aca="1" ref="P61" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B61)</f>
         <v>The cutting-edge Gorshkov frigates stick out in the largely-outdated Russian surface warfare fleet.</v>
       </c>
-      <c r="Q61" cm="1">
+      <c r="Q61" t="str" cm="1">
         <f t="array" aca="1" ref="Q61" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B61)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -8012,9 +8014,9 @@
         <f t="array" aca="1" ref="P62" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B62)</f>
         <v>With more than twice the firepower of western submarines, the Yasen is Russia's best effort in no-expense-spared attack submarine development.</v>
       </c>
-      <c r="Q62" cm="1">
+      <c r="Q62" t="str" cm="1">
         <f t="array" aca="1" ref="Q62" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B62)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -8081,9 +8083,9 @@
         <f t="array" aca="1" ref="P63" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B63)</f>
         <v>With more than twice the firepower of western submarines, the Yasen is Russia's best effort in no-expense-spared attack submarine development.</v>
       </c>
-      <c r="Q63" cm="1">
+      <c r="Q63" t="str" cm="1">
         <f t="array" aca="1" ref="Q63" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B63)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -8150,9 +8152,9 @@
         <f t="array" aca="1" ref="P64" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B64)</f>
         <v>With more than twice the firepower of western submarines, the Yasen is Russia's best effort in no-expense-spared attack submarine development.</v>
       </c>
-      <c r="Q64" cm="1">
+      <c r="Q64" t="str" cm="1">
         <f t="array" aca="1" ref="Q64" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B64)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -8219,9 +8221,9 @@
         <f t="array" aca="1" ref="P65" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B65)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q65" cm="1">
+      <c r="Q65" t="str" cm="1">
         <f t="array" aca="1" ref="Q65" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B65)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -8288,9 +8290,9 @@
         <f t="array" aca="1" ref="P66" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B66)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q66" cm="1">
+      <c r="Q66" t="str" cm="1">
         <f t="array" aca="1" ref="Q66" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B66)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -8357,9 +8359,9 @@
         <f t="array" aca="1" ref="P67" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B67)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q67" cm="1">
+      <c r="Q67" t="str" cm="1">
         <f t="array" aca="1" ref="Q67" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B67)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -8426,9 +8428,9 @@
         <f t="array" aca="1" ref="P68" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B68)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q68" cm="1">
+      <c r="Q68" t="str" cm="1">
         <f t="array" aca="1" ref="Q68" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B68)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -8495,9 +8497,9 @@
         <f t="array" aca="1" ref="P69" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B69)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q69" cm="1">
+      <c r="Q69" t="str" cm="1">
         <f t="array" aca="1" ref="Q69" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B69)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -8564,9 +8566,9 @@
         <f t="array" aca="1" ref="P70" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B70)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q70" cm="1">
+      <c r="Q70" t="str" cm="1">
         <f t="array" aca="1" ref="Q70" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B70)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8633,9 +8635,9 @@
         <f t="array" aca="1" ref="P71" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B71)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q71" cm="1">
+      <c r="Q71" t="str" cm="1">
         <f t="array" aca="1" ref="Q71" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B71)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -8702,9 +8704,9 @@
         <f t="array" aca="1" ref="P72" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B72)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q72" cm="1">
+      <c r="Q72" t="str" cm="1">
         <f t="array" aca="1" ref="Q72" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B72)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -8771,9 +8773,9 @@
         <f t="array" aca="1" ref="P73" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B73)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q73" cm="1">
+      <c r="Q73" t="str" cm="1">
         <f t="array" aca="1" ref="Q73" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B73)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8840,9 +8842,9 @@
         <f t="array" aca="1" ref="P74" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B74)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q74" cm="1">
+      <c r="Q74" t="str" cm="1">
         <f t="array" aca="1" ref="Q74" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B74)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -8909,9 +8911,9 @@
         <f t="array" aca="1" ref="P75" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B75)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q75" cm="1">
+      <c r="Q75" t="str" cm="1">
         <f t="array" aca="1" ref="Q75" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B75)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
@@ -8978,9 +8980,9 @@
         <f t="array" aca="1" ref="P76" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B76)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q76" cm="1">
+      <c r="Q76" t="str" cm="1">
         <f t="array" aca="1" ref="Q76" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B76)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -9047,9 +9049,9 @@
         <f t="array" aca="1" ref="P77" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B77)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q77" cm="1">
+      <c r="Q77" t="str" cm="1">
         <f t="array" aca="1" ref="Q77" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B77)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
@@ -9116,9 +9118,9 @@
         <f t="array" aca="1" ref="P78" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B78)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q78" cm="1">
+      <c r="Q78" t="str" cm="1">
         <f t="array" aca="1" ref="Q78" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B78)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -9185,9 +9187,9 @@
         <f t="array" aca="1" ref="P79" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B79)</f>
         <v>Although shorter-ranged than nuclear attack submarines, diesel-electric attack submarines are smaller, quieter and nearly as well armed.</v>
       </c>
-      <c r="Q79" cm="1">
+      <c r="Q79" t="str" cm="1">
         <f t="array" aca="1" ref="Q79" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B79)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -9254,9 +9256,9 @@
         <f t="array" aca="1" ref="P80" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B80)</f>
         <v>Although shorter-ranged than nuclear attack submarines, diesel-electric attack submarines are smaller, quieter and nearly as well armed.</v>
       </c>
-      <c r="Q80" cm="1">
+      <c r="Q80" t="str" cm="1">
         <f t="array" aca="1" ref="Q80" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B80)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
@@ -9322,9 +9324,9 @@
         <f t="array" aca="1" ref="P81" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B81)</f>
         <v>With a $15M unit cost conceivably affordable by even second-tier NBA starters, the Mig-29K is proof that performance and price are not always at odds.</v>
       </c>
-      <c r="Q81" cm="1">
+      <c r="Q81" t="str" cm="1">
         <f t="array" aca="1" ref="Q81" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B81)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
@@ -9390,9 +9392,9 @@
         <f t="array" aca="1" ref="P82" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B82)</f>
         <v>With a $15M unit cost conceivably affordable by even second-tier NBA starters, the Mig-29K is proof that performance and price are not always at odds.</v>
       </c>
-      <c r="Q82" cm="1">
+      <c r="Q82" t="str" cm="1">
         <f t="array" aca="1" ref="Q82" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B82)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
@@ -9458,9 +9460,9 @@
         <f t="array" aca="1" ref="P83" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B83)</f>
         <v>With a $15M unit cost conceivably affordable by even second-tier NBA starters, the Mig-29K is proof that performance and price are not always at odds.</v>
       </c>
-      <c r="Q83" cm="1">
+      <c r="Q83" t="str" cm="1">
         <f t="array" aca="1" ref="Q83" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B83)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
@@ -9541,9 +9543,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G3">
+      <c r="G3" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -9567,9 +9569,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G4">
+      <c r="G4" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -9600,9 +9602,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G6">
+      <c r="G6" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -9626,9 +9628,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G7">
+      <c r="G7" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -9652,9 +9654,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G8">
+      <c r="G8" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -9678,9 +9680,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G9">
+      <c r="G9" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -9704,9 +9706,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G10">
+      <c r="G10" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -9730,9 +9732,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G11">
+      <c r="G11" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -9763,9 +9765,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G13">
+      <c r="G13" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -9789,9 +9791,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G14">
+      <c r="G14" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9815,9 +9817,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G15">
+      <c r="G15" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9842,9 +9844,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G17">
+      <c r="G17" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -9868,9 +9870,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G18">
+      <c r="G18" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -9908,9 +9910,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G21">
+      <c r="G21" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -9934,9 +9936,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G22">
+      <c r="G22" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -9974,9 +9976,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G25">
+      <c r="G25" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -10000,9 +10002,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G26">
+      <c r="G26" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -10026,9 +10028,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G27">
+      <c r="G27" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -10052,9 +10054,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="G28">
+      <c r="G28" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -10067,7 +10069,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K25"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10161,9 +10163,9 @@
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K2" cm="1">
+      <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -10204,9 +10206,9 @@
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>Images/pearlharbor.jpg</v>
       </c>
-      <c r="K3" cm="1">
+      <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -10249,9 +10251,9 @@
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K4" cm="1">
+      <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -10294,9 +10296,9 @@
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K5" cm="1">
+      <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -10339,9 +10341,9 @@
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K6" cm="1">
+      <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -10384,9 +10386,9 @@
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K7" cm="1">
+      <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -10429,9 +10431,9 @@
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K8" cm="1">
+      <c r="K8" t="str" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -10474,9 +10476,9 @@
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K9" cm="1">
+      <c r="K9" t="str" cm="1">
         <f t="array" aca="1" ref="K9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -10519,9 +10521,9 @@
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K10" cm="1">
+      <c r="K10" t="str" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -10564,9 +10566,9 @@
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K11" cm="1">
+      <c r="K11" t="str" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -10608,9 +10610,9 @@
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
         <v>Images/pinegap.jpg</v>
       </c>
-      <c r="K12" cm="1">
+      <c r="K12" t="str" cm="1">
         <f t="array" aca="1" ref="K12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -10653,9 +10655,9 @@
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K13" cm="1">
+      <c r="K13" t="str" cm="1">
         <f t="array" aca="1" ref="K13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -10697,9 +10699,9 @@
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K14" cm="1">
+      <c r="K14" t="str" cm="1">
         <f t="array" aca="1" ref="K14" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -10741,9 +10743,9 @@
         <f t="array" aca="1" ref="J15" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K15" cm="1">
+      <c r="K15" t="str" cm="1">
         <f t="array" aca="1" ref="K15" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -10785,9 +10787,9 @@
         <f t="array" aca="1" ref="J16" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K16" cm="1">
+      <c r="K16" t="str" cm="1">
         <f t="array" aca="1" ref="K16" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -10829,9 +10831,9 @@
         <f t="array" aca="1" ref="J17" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K17" cm="1">
+      <c r="K17" t="str" cm="1">
         <f t="array" aca="1" ref="K17" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -10873,9 +10875,9 @@
         <f t="array" aca="1" ref="J18" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K18" cm="1">
+      <c r="K18" t="str" cm="1">
         <f t="array" aca="1" ref="K18" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -10917,9 +10919,9 @@
         <f t="array" aca="1" ref="J19" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K19" cm="1">
+      <c r="K19" t="str" cm="1">
         <f t="array" aca="1" ref="K19" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -10961,9 +10963,9 @@
         <f t="array" aca="1" ref="J20" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K20" cm="1">
+      <c r="K20" t="str" cm="1">
         <f t="array" aca="1" ref="K20" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -11005,9 +11007,9 @@
         <f t="array" aca="1" ref="J21" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K21" cm="1">
+      <c r="K21" t="str" cm="1">
         <f t="array" aca="1" ref="K21" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -11049,9 +11051,9 @@
         <f t="array" aca="1" ref="J22" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K22" cm="1">
+      <c r="K22" t="str" cm="1">
         <f t="array" aca="1" ref="K22" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -11093,9 +11095,9 @@
         <f t="array" aca="1" ref="J23" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K23" cm="1">
+      <c r="K23" t="str" cm="1">
         <f t="array" aca="1" ref="K23" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -11137,9 +11139,9 @@
         <f t="array" aca="1" ref="J24" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K24" cm="1">
+      <c r="K24" t="str" cm="1">
         <f t="array" aca="1" ref="K24" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -11181,9 +11183,9 @@
         <f t="array" aca="1" ref="J25" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K25" cm="1">
+      <c r="K25" t="str" cm="1">
         <f t="array" aca="1" ref="K25" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -11287,9 +11289,9 @@
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K2" cm="1">
+      <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -11330,9 +11332,9 @@
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>Images/pearlharbor.jpg</v>
       </c>
-      <c r="K3" cm="1">
+      <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -11375,9 +11377,9 @@
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K4" cm="1">
+      <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -11420,9 +11422,9 @@
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K5" cm="1">
+      <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -11465,9 +11467,9 @@
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K6" cm="1">
+      <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -11510,9 +11512,9 @@
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K7" cm="1">
+      <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -11555,9 +11557,9 @@
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K8" cm="1">
+      <c r="K8" t="str" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -11600,9 +11602,9 @@
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K9" cm="1">
+      <c r="K9" t="str" cm="1">
         <f t="array" aca="1" ref="K9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -11645,9 +11647,9 @@
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K10" cm="1">
+      <c r="K10" t="str" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -11690,9 +11692,9 @@
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K11" cm="1">
+      <c r="K11" t="str" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -11734,9 +11736,9 @@
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
         <v>Images/pinegap.jpg</v>
       </c>
-      <c r="K12" cm="1">
+      <c r="K12" t="str" cm="1">
         <f t="array" aca="1" ref="K12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -11779,9 +11781,9 @@
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
         <v>Images/navalbase.jpg</v>
       </c>
-      <c r="K13" cm="1">
+      <c r="K13" t="str" cm="1">
         <f t="array" aca="1" ref="K13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -11881,9 +11883,9 @@
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K2" cm="1">
+      <c r="K2" t="str" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -11925,9 +11927,9 @@
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K3" cm="1">
+      <c r="K3" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -11969,9 +11971,9 @@
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K4" cm="1">
+      <c r="K4" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -12013,9 +12015,9 @@
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K5" cm="1">
+      <c r="K5" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -12057,9 +12059,9 @@
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K6" cm="1">
+      <c r="K6" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -12101,9 +12103,9 @@
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K7" cm="1">
+      <c r="K7" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -12145,9 +12147,9 @@
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K8" cm="1">
+      <c r="K8" t="str" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -12189,9 +12191,9 @@
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K9" cm="1">
+      <c r="K9" t="str" cm="1">
         <f t="array" aca="1" ref="K9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -12233,9 +12235,9 @@
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K10" cm="1">
+      <c r="K10" t="str" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -12277,9 +12279,9 @@
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K11" cm="1">
+      <c r="K11" t="str" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -12321,9 +12323,9 @@
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K12" cm="1">
+      <c r="K12" t="str" cm="1">
         <f t="array" aca="1" ref="K12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -12365,9 +12367,9 @@
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
         <v>Images/russnavybase.jpg</v>
       </c>
-      <c r="K13" cm="1">
+      <c r="K13" t="str" cm="1">
         <f t="array" aca="1" ref="K13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -12446,9 +12448,9 @@
       <c r="G2" t="s">
         <v>222</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12476,9 +12478,9 @@
       <c r="G3" t="s">
         <v>224</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12504,9 +12506,9 @@
       <c r="G4" t="s">
         <v>317</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -12534,9 +12536,9 @@
       <c r="G5" t="s">
         <v>223</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14958,9 +14960,9 @@
         <f t="array" aca="1" ref="P2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>A military airbase at sea, a Nimitz carrier is more than three times as long as a football field and has more than twice the displacement of the German super-battleship Bismarck.</v>
       </c>
-      <c r="Q2" cm="1">
+      <c r="Q2" t="str" cm="1">
         <f t="array" aca="1" ref="Q2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -15027,9 +15029,9 @@
         <f t="array" aca="1" ref="P3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>A military airbase at sea, a Nimitz carrier is more than three times as long as a football field and has more than twice the displacement of the German super-battleship Bismarck.</v>
       </c>
-      <c r="Q3" cm="1">
+      <c r="Q3" t="str" cm="1">
         <f t="array" aca="1" ref="Q3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -15096,9 +15098,9 @@
         <f t="array" aca="1" ref="P4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>A military airbase at sea, a Nimitz carrier is more than three times as long as a football field and has more than twice the displacement of the German super-battleship Bismarck.</v>
       </c>
-      <c r="Q4" cm="1">
+      <c r="Q4" t="str" cm="1">
         <f t="array" aca="1" ref="Q4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -15164,9 +15166,9 @@
         <f t="array" aca="1" ref="P5" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q5" cm="1">
+      <c r="Q5" t="str" cm="1">
         <f t="array" aca="1" ref="Q5" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -15232,9 +15234,9 @@
         <f t="array" aca="1" ref="P6" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q6" cm="1">
+      <c r="Q6" t="str" cm="1">
         <f t="array" aca="1" ref="Q6" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -15300,9 +15302,9 @@
         <f t="array" aca="1" ref="P7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q7" cm="1">
+      <c r="Q7" t="str" cm="1">
         <f t="array" aca="1" ref="Q7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -15368,9 +15370,9 @@
         <f t="array" aca="1" ref="P8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q8" cm="1">
+      <c r="Q8" t="str" cm="1">
         <f t="array" aca="1" ref="Q8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -15436,9 +15438,9 @@
         <f t="array" aca="1" ref="P9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
         <v>In addition to supporting VTOL aircraft, a Wasp amphibious assault ship is capable of delivering a Marine Expeditionary Unit complete with its armored vehicles to hostile shores via helicopters and landing craft.</v>
       </c>
-      <c r="Q9" cm="1">
+      <c r="Q9" t="str" cm="1">
         <f t="array" aca="1" ref="Q9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -15506,9 +15508,9 @@
         <f t="array" aca="1" ref="P10" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
         <v>As the most expensive class of attack submarine ever built, the Seawolf is the apex predator of the US Navy's submarine fleet.</v>
       </c>
-      <c r="Q10" cm="1">
+      <c r="Q10" t="str" cm="1">
         <f t="array" aca="1" ref="Q10" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -15575,9 +15577,9 @@
         <f t="array" aca="1" ref="P11" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
         <v>The advanced Virginia will be the standard attack submarine of the US Navy until at least the middle of the 21st century.</v>
       </c>
-      <c r="Q11" cm="1">
+      <c r="Q11" t="str" cm="1">
         <f t="array" aca="1" ref="Q11" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -15644,9 +15646,9 @@
         <f t="array" aca="1" ref="P12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
         <v>The advanced Virginia will be the standard attack submarine of the US Navy until at least the middle of the 21st century.</v>
       </c>
-      <c r="Q12" cm="1">
+      <c r="Q12" t="str" cm="1">
         <f t="array" aca="1" ref="Q12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -15713,9 +15715,9 @@
         <f t="array" aca="1" ref="P13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
         <v>The advanced Virginia will be the standard attack submarine of the US Navy until at least the middle of the 21st century.</v>
       </c>
-      <c r="Q13" cm="1">
+      <c r="Q13" t="str" cm="1">
         <f t="array" aca="1" ref="Q13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -15782,9 +15784,9 @@
         <f t="array" aca="1" ref="P14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
         <v>Although Ohio was originally intended to carry nuclear ballistic missiles, some Ohio's have been modified as SSGNs for surface warfare and land-attack missions.</v>
       </c>
-      <c r="Q14" cm="1">
+      <c r="Q14" t="str" cm="1">
         <f t="array" aca="1" ref="Q14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -15851,9 +15853,9 @@
         <f t="array" aca="1" ref="P15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
         <v>Although Ohio was originally intended to carry nuclear ballistic missiles, some Ohio's have been modified as SSGNs for surface warfare and land-attack missions.</v>
       </c>
-      <c r="Q15" cm="1">
+      <c r="Q15" t="str" cm="1">
         <f t="array" aca="1" ref="Q15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -15918,9 +15920,9 @@
         <f t="array" aca="1" ref="P16" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
         <v>Despite a modest displacement by historical standards, the Ticonderoga is the largest surface combatant in the US Navy.</v>
       </c>
-      <c r="Q16" cm="1">
+      <c r="Q16" t="str" cm="1">
         <f t="array" aca="1" ref="Q16" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -15985,9 +15987,9 @@
         <f t="array" aca="1" ref="P17" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
         <v>Despite a modest displacement by historical standards, the Ticonderoga is the largest surface combatant in the US Navy.</v>
       </c>
-      <c r="Q17" cm="1">
+      <c r="Q17" t="str" cm="1">
         <f t="array" aca="1" ref="Q17" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -16052,9 +16054,9 @@
         <f t="array" aca="1" ref="P18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
         <v>Despite a modest displacement by historical standards, the Ticonderoga is the largest surface combatant in the US Navy.</v>
       </c>
-      <c r="Q18" cm="1">
+      <c r="Q18" t="str" cm="1">
         <f t="array" aca="1" ref="Q18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -16119,9 +16121,9 @@
         <f t="array" aca="1" ref="P19" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q19" cm="1">
+      <c r="Q19" t="str" cm="1">
         <f t="array" aca="1" ref="Q19" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -16186,9 +16188,9 @@
         <f t="array" aca="1" ref="P20" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q20" cm="1">
+      <c r="Q20" t="str" cm="1">
         <f t="array" aca="1" ref="Q20" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -16253,9 +16255,9 @@
         <f t="array" aca="1" ref="P21" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q21" cm="1">
+      <c r="Q21" t="str" cm="1">
         <f t="array" aca="1" ref="Q21" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -16320,9 +16322,9 @@
         <f t="array" aca="1" ref="P22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q22" cm="1">
+      <c r="Q22" t="str" cm="1">
         <f t="array" aca="1" ref="Q22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -16387,9 +16389,9 @@
         <f t="array" aca="1" ref="P23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
         <v>The multi-mission Arleigh Burke is the most numerous ship in the US Navy.</v>
       </c>
-      <c r="Q23" cm="1">
+      <c r="Q23" t="str" cm="1">
         <f t="array" aca="1" ref="Q23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -16454,9 +16456,9 @@
         <f t="array" aca="1" ref="P24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
         <v>With a cost of $1M per shot from its main howitzer, it is important for the crew of a Zumwalt to aim carefully.</v>
       </c>
-      <c r="Q24" cm="1">
+      <c r="Q24" t="str" cm="1">
         <f t="array" aca="1" ref="Q24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -16521,9 +16523,9 @@
         <f t="array" aca="1" ref="P25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
         <v>With a cost of $1M per shot from its main howitzer, it is important for the crew of a Zumwalt to aim carefully.</v>
       </c>
-      <c r="Q25" cm="1">
+      <c r="Q25" t="str" cm="1">
         <f t="array" aca="1" ref="Q25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -16589,9 +16591,9 @@
         <f t="array" aca="1" ref="P26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q26" cm="1">
+      <c r="Q26" t="str" cm="1">
         <f t="array" aca="1" ref="Q26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -16657,9 +16659,9 @@
         <f t="array" aca="1" ref="P27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q27" cm="1">
+      <c r="Q27" t="str" cm="1">
         <f t="array" aca="1" ref="Q27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -16725,9 +16727,9 @@
         <f t="array" aca="1" ref="P28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q28" cm="1">
+      <c r="Q28" t="str" cm="1">
         <f t="array" aca="1" ref="Q28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -16793,9 +16795,9 @@
         <f t="array" aca="1" ref="P29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q29" cm="1">
+      <c r="Q29" t="str" cm="1">
         <f t="array" aca="1" ref="Q29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -16861,9 +16863,9 @@
         <f t="array" aca="1" ref="P30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
         <v>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</v>
       </c>
-      <c r="Q30" cm="1">
+      <c r="Q30" t="str" cm="1">
         <f t="array" aca="1" ref="Q30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -16930,9 +16932,9 @@
         <f t="array" aca="1" ref="P31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
         <v>The F-35B is a special variant of the F-35 capable of taking off and landing vertically. This allows it to be stationed on smaller carriers that have typically not been able to field cutting-edge aircraft.</v>
       </c>
-      <c r="Q31" cm="1">
+      <c r="Q31" t="str" cm="1">
         <f t="array" aca="1" ref="Q31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -16999,9 +17001,9 @@
         <f t="array" aca="1" ref="P32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
         <v>The F-35B is a special variant of the F-35 capable of taking off and landing vertically. This allows it to be stationed on smaller carriers that have typically not been able to field cutting-edge aircraft.</v>
       </c>
-      <c r="Q32" cm="1">
+      <c r="Q32" t="str" cm="1">
         <f t="array" aca="1" ref="Q32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -17068,9 +17070,9 @@
         <f t="array" aca="1" ref="P33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
         <v>The F-35B is a special variant of the F-35 capable of taking off and landing vertically. This allows it to be stationed on smaller carriers that have typically not been able to field cutting-edge aircraft.</v>
       </c>
-      <c r="Q33" cm="1">
+      <c r="Q33" t="str" cm="1">
         <f t="array" aca="1" ref="Q33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -17137,9 +17139,9 @@
         <f t="array" aca="1" ref="P34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
         <v>The F-35 acquisition program cost of just under $450 billion USD would be enough to buy 450 billion $1 cheeseburgers - enough to kill all humans on earth.</v>
       </c>
-      <c r="Q34" cm="1">
+      <c r="Q34" t="str" cm="1">
         <f t="array" aca="1" ref="Q34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -17206,9 +17208,9 @@
         <f t="array" aca="1" ref="P35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
         <v>The F-35 acquisition program cost of just under $450 billion USD would be enough to buy 450 billion $1 cheeseburgers - enough to kill all humans on earth.</v>
       </c>
-      <c r="Q35" cm="1">
+      <c r="Q35" t="str" cm="1">
         <f t="array" aca="1" ref="Q35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -17275,9 +17277,9 @@
         <f t="array" aca="1" ref="P36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
         <v>The F-35 acquisition program cost of just under $450 billion USD would be enough to buy 450 billion $1 cheeseburgers - enough to kill all humans on earth.</v>
       </c>
-      <c r="Q36" cm="1">
+      <c r="Q36" t="str" cm="1">
         <f t="array" aca="1" ref="Q36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -17343,9 +17345,9 @@
         <f t="array" aca="1" ref="P37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q37" cm="1">
+      <c r="Q37" t="str" cm="1">
         <f t="array" aca="1" ref="Q37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -17411,9 +17413,9 @@
         <f t="array" aca="1" ref="P38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q38" cm="1">
+      <c r="Q38" t="str" cm="1">
         <f t="array" aca="1" ref="Q38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -17479,9 +17481,9 @@
         <f t="array" aca="1" ref="P39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q39" cm="1">
+      <c r="Q39" t="str" cm="1">
         <f t="array" aca="1" ref="Q39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -17547,9 +17549,9 @@
         <f t="array" aca="1" ref="P40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q40" cm="1">
+      <c r="Q40" t="str" cm="1">
         <f t="array" aca="1" ref="Q40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -17615,9 +17617,9 @@
         <f t="array" aca="1" ref="P41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
         <v>A Pepsi ad campaign promised to award a Harrier to anyone who collected enough Pepsi points- a promise Pepsi did not keep. During its service history, the Harrier has proven it is more reliable than Pepsi Co.</v>
       </c>
-      <c r="Q41" cm="1">
+      <c r="Q41" t="str" cm="1">
         <f t="array" aca="1" ref="Q41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -17894,9 +17896,9 @@
         <f t="array" aca="1" ref="P2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>Although sold to a company in Macau supposedly for use as a floating casino, Kuznetsov's sister ship has since unsurprisingly become the first aircraft carrier of the Chinese People's Liberation Army Navy.</v>
       </c>
-      <c r="Q2" cm="1">
+      <c r="Q2" t="str" cm="1">
         <f t="array" aca="1" ref="Q2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -17961,9 +17963,9 @@
         <f t="array" aca="1" ref="P3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>Since the decommisioning of the last retrofitted WWII-era battleship in 1991, the Kirov has been the largest surface combatant in the world.</v>
       </c>
-      <c r="Q3" cm="1">
+      <c r="Q3" t="str" cm="1">
         <f t="array" aca="1" ref="Q3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -18028,9 +18030,9 @@
         <f t="array" aca="1" ref="P4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>Since the decommisioning of the last retrofitted WWII-era battleship in 1991, the Kirov has been the largest surface combatant in the world.</v>
       </c>
-      <c r="Q4" cm="1">
+      <c r="Q4" t="str" cm="1">
         <f t="array" aca="1" ref="Q4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -18095,9 +18097,9 @@
         <f t="array" aca="1" ref="P5" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
         <v>Since the decommisioning of the last retrofitted WWII-era battleship in 1991, the Kirov has been the largest surface combatant in the world.</v>
       </c>
-      <c r="Q5" cm="1">
+      <c r="Q5" t="str" cm="1">
         <f t="array" aca="1" ref="Q5" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -18162,9 +18164,9 @@
         <f t="array" aca="1" ref="P6" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q6" cm="1">
+      <c r="Q6" t="str" cm="1">
         <f t="array" aca="1" ref="Q6" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -18229,9 +18231,9 @@
         <f t="array" aca="1" ref="P7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q7" cm="1">
+      <c r="Q7" t="str" cm="1">
         <f t="array" aca="1" ref="Q7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -18296,9 +18298,9 @@
         <f t="array" aca="1" ref="P8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q8" cm="1">
+      <c r="Q8" t="str" cm="1">
         <f t="array" aca="1" ref="Q8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -18363,9 +18365,9 @@
         <f t="array" aca="1" ref="P9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
         <v>Equipped with the same massive anti-ship missiles as the Kirov class, the Slava packs a similar punch in a considerably smaller form-factor.</v>
       </c>
-      <c r="Q9" cm="1">
+      <c r="Q9" t="str" cm="1">
         <f t="array" aca="1" ref="Q9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -18431,9 +18433,9 @@
         <f t="array" aca="1" ref="P10" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q10" cm="1">
+      <c r="Q10" t="str" cm="1">
         <f t="array" aca="1" ref="Q10" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -18499,9 +18501,9 @@
         <f t="array" aca="1" ref="P11" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q11" cm="1">
+      <c r="Q11" t="str" cm="1">
         <f t="array" aca="1" ref="Q11" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -18567,9 +18569,9 @@
         <f t="array" aca="1" ref="P12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q12" cm="1">
+      <c r="Q12" t="str" cm="1">
         <f t="array" aca="1" ref="Q12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -18635,9 +18637,9 @@
         <f t="array" aca="1" ref="P13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q13" cm="1">
+      <c r="Q13" t="str" cm="1">
         <f t="array" aca="1" ref="Q13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -18703,9 +18705,9 @@
         <f t="array" aca="1" ref="P14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q14" cm="1">
+      <c r="Q14" t="str" cm="1">
         <f t="array" aca="1" ref="Q14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -18771,9 +18773,9 @@
         <f t="array" aca="1" ref="P15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
         <v>Udaloy II: the ship so nice they designed it twice.</v>
       </c>
-      <c r="Q15" cm="1">
+      <c r="Q15" t="str" cm="1">
         <f t="array" aca="1" ref="Q15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -18839,9 +18841,9 @@
         <f t="array" aca="1" ref="P16" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q16" cm="1">
+      <c r="Q16" t="str" cm="1">
         <f t="array" aca="1" ref="Q16" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -18907,9 +18909,9 @@
         <f t="array" aca="1" ref="P17" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q17" cm="1">
+      <c r="Q17" t="str" cm="1">
         <f t="array" aca="1" ref="Q17" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -18975,9 +18977,9 @@
         <f t="array" aca="1" ref="P18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q18" cm="1">
+      <c r="Q18" t="str" cm="1">
         <f t="array" aca="1" ref="Q18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -19043,9 +19045,9 @@
         <f t="array" aca="1" ref="P19" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
         <v>With a name that means "modern" in Russian, they are the oldest class of destroyer in the Russian Navy.</v>
       </c>
-      <c r="Q19" cm="1">
+      <c r="Q19" t="str" cm="1">
         <f t="array" aca="1" ref="Q19" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -19110,9 +19112,9 @@
         <f t="array" aca="1" ref="P20" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
         <v>The cutting-edge Gorshkov frigates stick out in the largely-outdated Russian surface warfare fleet.</v>
       </c>
-      <c r="Q20" cm="1">
+      <c r="Q20" t="str" cm="1">
         <f t="array" aca="1" ref="Q20" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -19177,9 +19179,9 @@
         <f t="array" aca="1" ref="P21" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
         <v>The cutting-edge Gorshkov frigates stick out in the largely-outdated Russian surface warfare fleet.</v>
       </c>
-      <c r="Q21" cm="1">
+      <c r="Q21" t="str" cm="1">
         <f t="array" aca="1" ref="Q21" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -19246,9 +19248,9 @@
         <f t="array" aca="1" ref="P22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
         <v>With more than twice the firepower of western submarines, the Yasen is Russia's best effort in no-expense-spared attack submarine development.</v>
       </c>
-      <c r="Q22" cm="1">
+      <c r="Q22" t="str" cm="1">
         <f t="array" aca="1" ref="Q22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -19315,9 +19317,9 @@
         <f t="array" aca="1" ref="P23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
         <v>With more than twice the firepower of western submarines, the Yasen is Russia's best effort in no-expense-spared attack submarine development.</v>
       </c>
-      <c r="Q23" cm="1">
+      <c r="Q23" t="str" cm="1">
         <f t="array" aca="1" ref="Q23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -19384,9 +19386,9 @@
         <f t="array" aca="1" ref="P24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
         <v>With more than twice the firepower of western submarines, the Yasen is Russia's best effort in no-expense-spared attack submarine development.</v>
       </c>
-      <c r="Q24" cm="1">
+      <c r="Q24" t="str" cm="1">
         <f t="array" aca="1" ref="Q24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -19453,9 +19455,9 @@
         <f t="array" aca="1" ref="P25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q25" cm="1">
+      <c r="Q25" t="str" cm="1">
         <f t="array" aca="1" ref="Q25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -19522,9 +19524,9 @@
         <f t="array" aca="1" ref="P26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q26" cm="1">
+      <c r="Q26" t="str" cm="1">
         <f t="array" aca="1" ref="Q26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -19591,9 +19593,9 @@
         <f t="array" aca="1" ref="P27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q27" cm="1">
+      <c r="Q27" t="str" cm="1">
         <f t="array" aca="1" ref="Q27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -19660,9 +19662,9 @@
         <f t="array" aca="1" ref="P28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
         <v>The massive but aging Oscar is a relic of Cold War Soviet strategy. That said, it's large guided missile batteries are still a formidable threat to US carriers.</v>
       </c>
-      <c r="Q28" cm="1">
+      <c r="Q28" t="str" cm="1">
         <f t="array" aca="1" ref="Q28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -19729,9 +19731,9 @@
         <f t="array" aca="1" ref="P29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q29" cm="1">
+      <c r="Q29" t="str" cm="1">
         <f t="array" aca="1" ref="Q29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -19798,9 +19800,9 @@
         <f t="array" aca="1" ref="P30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q30" cm="1">
+      <c r="Q30" t="str" cm="1">
         <f t="array" aca="1" ref="Q30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -19867,9 +19869,9 @@
         <f t="array" aca="1" ref="P31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q31" cm="1">
+      <c r="Q31" t="str" cm="1">
         <f t="array" aca="1" ref="Q31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -19936,9 +19938,9 @@
         <f t="array" aca="1" ref="P32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q32" cm="1">
+      <c r="Q32" t="str" cm="1">
         <f t="array" aca="1" ref="Q32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -20005,9 +20007,9 @@
         <f t="array" aca="1" ref="P33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q33" cm="1">
+      <c r="Q33" t="str" cm="1">
         <f t="array" aca="1" ref="Q33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -20074,9 +20076,9 @@
         <f t="array" aca="1" ref="P34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
         <v>In Russian, akula means shark</v>
       </c>
-      <c r="Q34" cm="1">
+      <c r="Q34" t="str" cm="1">
         <f t="array" aca="1" ref="Q34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -20143,9 +20145,9 @@
         <f t="array" aca="1" ref="P35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q35" cm="1">
+      <c r="Q35" t="str" cm="1">
         <f t="array" aca="1" ref="Q35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -20212,9 +20214,9 @@
         <f t="array" aca="1" ref="P36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q36" cm="1">
+      <c r="Q36" t="str" cm="1">
         <f t="array" aca="1" ref="Q36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -20281,9 +20283,9 @@
         <f t="array" aca="1" ref="P37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q37" cm="1">
+      <c r="Q37" t="str" cm="1">
         <f t="array" aca="1" ref="Q37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -20350,9 +20352,9 @@
         <f t="array" aca="1" ref="P38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
         <v>Nothing fancy, but it ain't bad for government work.</v>
       </c>
-      <c r="Q38" cm="1">
+      <c r="Q38" t="str" cm="1">
         <f t="array" aca="1" ref="Q38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -20419,9 +20421,9 @@
         <f t="array" aca="1" ref="P39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
         <v>Although shorter-ranged than nuclear attack submarines, diesel-electric attack submarines are smaller, quieter and nearly as well armed.</v>
       </c>
-      <c r="Q39" cm="1">
+      <c r="Q39" t="str" cm="1">
         <f t="array" aca="1" ref="Q39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -20488,9 +20490,9 @@
         <f t="array" aca="1" ref="P40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
         <v>Although shorter-ranged than nuclear attack submarines, diesel-electric attack submarines are smaller, quieter and nearly as well armed.</v>
       </c>
-      <c r="Q40" cm="1">
+      <c r="Q40" t="str" cm="1">
         <f t="array" aca="1" ref="Q40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -20556,9 +20558,9 @@
         <f t="array" aca="1" ref="P41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
         <v>With a $15M unit cost conceivably affordable by even second-tier NBA starters, the Mig-29K is proof that performance and price are not always at odds.</v>
       </c>
-      <c r="Q41" cm="1">
+      <c r="Q41" t="str" cm="1">
         <f t="array" aca="1" ref="Q41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -20624,9 +20626,9 @@
         <f t="array" aca="1" ref="P42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
         <v>With a $15M unit cost conceivably affordable by even second-tier NBA starters, the Mig-29K is proof that performance and price are not always at odds.</v>
       </c>
-      <c r="Q42" cm="1">
+      <c r="Q42" t="str" cm="1">
         <f t="array" aca="1" ref="Q42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -20692,9 +20694,9 @@
         <f t="array" aca="1" ref="P43" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B43)</f>
         <v>With a $15M unit cost conceivably affordable by even second-tier NBA starters, the Mig-29K is proof that performance and price are not always at odds.</v>
       </c>
-      <c r="Q43" cm="1">
+      <c r="Q43" t="str" cm="1">
         <f t="array" aca="1" ref="Q43" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B43)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -20706,9 +20708,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA93C54-FC77-4A57-AEDF-D4D1B82432EF}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20804,9 +20806,9 @@
       <c r="M2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -20840,9 +20842,9 @@
       <c r="L3" t="s">
         <v>78</v>
       </c>
-      <c r="N3">
+      <c r="N3" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -20878,9 +20880,9 @@
       <c r="M4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="N4">
+      <c r="N4" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -20913,9 +20915,9 @@
       <c r="L5" t="s">
         <v>80</v>
       </c>
-      <c r="N5">
+      <c r="N5" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20953,9 +20955,9 @@
       <c r="M6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N6">
+      <c r="N6" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -20992,9 +20994,9 @@
       <c r="M7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="N7">
+      <c r="N7" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21031,9 +21033,9 @@
       <c r="M8" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N8">
+      <c r="N8" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21068,9 +21070,9 @@
       <c r="M9" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="N9">
+      <c r="N9" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21105,9 +21107,9 @@
       <c r="M10" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="N10">
+      <c r="N10" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -21142,9 +21144,9 @@
       <c r="M11" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="N11">
+      <c r="N11" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21180,9 +21182,9 @@
       <c r="M12" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="N12">
+      <c r="N12" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21219,9 +21221,9 @@
       <c r="M13" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="N13">
+      <c r="N13" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -21258,9 +21260,9 @@
       <c r="M14" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="N14">
+      <c r="N14" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="78" customHeight="1" x14ac:dyDescent="0.25">
@@ -21296,9 +21298,9 @@
       <c r="M15" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="N15">
+      <c r="N15" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -21334,9 +21336,9 @@
       <c r="M16" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N16">
+      <c r="N16" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -21371,9 +21373,9 @@
       <c r="M17" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="N17">
+      <c r="N17" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -21408,9 +21410,9 @@
       <c r="M18" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N18">
+      <c r="N18" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21446,9 +21448,9 @@
       <c r="M19" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="N19">
+      <c r="N19" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21483,9 +21485,9 @@
       <c r="M20" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="N20">
+      <c r="N20" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21522,9 +21524,9 @@
       <c r="M21" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="N21">
+      <c r="N21" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -21561,9 +21563,9 @@
       <c r="M22" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="N22">
+      <c r="N22" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -21600,9 +21602,9 @@
       <c r="M23" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="N23">
+      <c r="N23" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -21638,9 +21640,9 @@
       <c r="M24" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="N24">
+      <c r="N24" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21676,9 +21678,9 @@
       <c r="M25" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="N25">
+      <c r="N25" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21715,9 +21717,9 @@
       <c r="M26" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="N26">
+      <c r="N26" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -21754,9 +21756,9 @@
       <c r="M27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="N27">
+      <c r="N27" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -21792,9 +21794,9 @@
       <c r="M28" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="N28">
+      <c r="N28" t="str">
         <f>version!$A$1</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -22000,8 +22002,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1.7</v>
+      <c r="A1" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -22014,7 +22016,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J24"/>
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22101,9 +22103,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J2" cm="1">
+      <c r="J2" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -22141,9 +22143,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J3" cm="1">
+      <c r="J3" t="str" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -22181,9 +22183,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J4" cm="1">
+      <c r="J4" t="str" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -22221,9 +22223,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J5" cm="1">
+      <c r="J5" t="str" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -22261,9 +22263,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J6" cm="1">
+      <c r="J6" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -22301,9 +22303,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J7" cm="1">
+      <c r="J7" t="str" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -22341,9 +22343,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J8" cm="1">
+      <c r="J8" t="str" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -22381,9 +22383,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J9" cm="1">
+      <c r="J9" t="str" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -22421,9 +22423,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J10" cm="1">
+      <c r="J10" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -22461,9 +22463,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J11" cm="1">
+      <c r="J11" t="str" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -22501,9 +22503,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J12" cm="1">
+      <c r="J12" t="str" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -22541,9 +22543,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J13" cm="1">
+      <c r="J13" t="str" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -22581,9 +22583,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J14" cm="1">
+      <c r="J14" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -22621,9 +22623,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J15" cm="1">
+      <c r="J15" t="str" cm="1">
         <f t="array" aca="1" ref="J15" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -22661,9 +22663,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J16" cm="1">
+      <c r="J16" t="str" cm="1">
         <f t="array" aca="1" ref="J16" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -22701,9 +22703,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J17" cm="1">
+      <c r="J17" t="str" cm="1">
         <f t="array" aca="1" ref="J17" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -22741,9 +22743,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J18" cm="1">
+      <c r="J18" t="str" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -22781,9 +22783,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J19" cm="1">
+      <c r="J19" t="str" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -22821,9 +22823,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J20" cm="1">
+      <c r="J20" t="str" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -22861,9 +22863,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J21" cm="1">
+      <c r="J21" t="str" cm="1">
         <f t="array" aca="1" ref="J21" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -22901,9 +22903,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J22" cm="1">
+      <c r="J22" t="str" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -22941,9 +22943,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J23" cm="1">
+      <c r="J23" t="str" cm="1">
         <f t="array" aca="1" ref="J23" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -22981,9 +22983,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J24" cm="1">
+      <c r="J24" t="str" cm="1">
         <f t="array" aca="1" ref="J24" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -23021,9 +23023,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J25" cm="1">
+      <c r="J25" t="str" cm="1">
         <f t="array" aca="1" ref="J25" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -23061,9 +23063,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J26" cm="1">
+      <c r="J26" t="str" cm="1">
         <f t="array" aca="1" ref="J26" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -23101,9 +23103,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J27" cm="1">
+      <c r="J27" t="str" cm="1">
         <f t="array" aca="1" ref="J27" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -23141,9 +23143,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J28" cm="1">
+      <c r="J28" t="str" cm="1">
         <f t="array" aca="1" ref="J28" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -23181,9 +23183,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J29" cm="1">
+      <c r="J29" t="str" cm="1">
         <f t="array" aca="1" ref="J29" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -23221,9 +23223,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J30" cm="1">
+      <c r="J30" t="str" cm="1">
         <f t="array" aca="1" ref="J30" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -23261,9 +23263,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J31" cm="1">
+      <c r="J31" t="str" cm="1">
         <f t="array" aca="1" ref="J31" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -23301,9 +23303,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J32" cm="1">
+      <c r="J32" t="str" cm="1">
         <f t="array" aca="1" ref="J32" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -23341,9 +23343,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J33" cm="1">
+      <c r="J33" t="str" cm="1">
         <f t="array" aca="1" ref="J33" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -23381,9 +23383,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J34" cm="1">
+      <c r="J34" t="str" cm="1">
         <f t="array" aca="1" ref="J34" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -23421,9 +23423,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J35" cm="1">
+      <c r="J35" t="str" cm="1">
         <f t="array" aca="1" ref="J35" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -23461,9 +23463,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J36" cm="1">
+      <c r="J36" t="str" cm="1">
         <f t="array" aca="1" ref="J36" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -23501,9 +23503,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J37" cm="1">
+      <c r="J37" t="str" cm="1">
         <f t="array" aca="1" ref="J37" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -23541,9 +23543,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J38" cm="1">
+      <c r="J38" t="str" cm="1">
         <f t="array" aca="1" ref="J38" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -23581,9 +23583,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J39" cm="1">
+      <c r="J39" t="str" cm="1">
         <f t="array" aca="1" ref="J39" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -23621,9 +23623,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J40" cm="1">
+      <c r="J40" t="str" cm="1">
         <f t="array" aca="1" ref="J40" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -23661,9 +23663,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J41" cm="1">
+      <c r="J41" t="str" cm="1">
         <f t="array" aca="1" ref="J41" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -23701,9 +23703,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J42" cm="1">
+      <c r="J42" t="str" cm="1">
         <f t="array" aca="1" ref="J42" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -23741,9 +23743,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J43" cm="1">
+      <c r="J43" t="str" cm="1">
         <f t="array" aca="1" ref="J43" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B43)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -23781,9 +23783,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J44" cm="1">
+      <c r="J44" t="str" cm="1">
         <f t="array" aca="1" ref="J44" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B44)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -23821,9 +23823,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J45" cm="1">
+      <c r="J45" t="str" cm="1">
         <f t="array" aca="1" ref="J45" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B45)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -23835,7 +23837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED05A72-9DE0-4247-9F2F-531B551ED433}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -23918,9 +23920,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J2" cm="1">
+      <c r="J2" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -23958,9 +23960,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J3" cm="1">
+      <c r="J3" t="str" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -23998,9 +24000,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J4" cm="1">
+      <c r="J4" t="str" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -24038,9 +24040,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J5" cm="1">
+      <c r="J5" t="str" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -24078,9 +24080,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J6" cm="1">
+      <c r="J6" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -24118,9 +24120,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J7" cm="1">
+      <c r="J7" t="str" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -24158,9 +24160,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J8" cm="1">
+      <c r="J8" t="str" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -24198,9 +24200,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J9" cm="1">
+      <c r="J9" t="str" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -24238,9 +24240,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J10" cm="1">
+      <c r="J10" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -24278,9 +24280,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J11" cm="1">
+      <c r="J11" t="str" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -24318,9 +24320,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J12" cm="1">
+      <c r="J12" t="str" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -24358,9 +24360,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J13" cm="1">
+      <c r="J13" t="str" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -24398,9 +24400,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J14" cm="1">
+      <c r="J14" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -24438,9 +24440,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J15" cm="1">
+      <c r="J15" t="str" cm="1">
         <f t="array" aca="1" ref="J15" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -24478,9 +24480,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J16" cm="1">
+      <c r="J16" t="str" cm="1">
         <f t="array" aca="1" ref="J16" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -24518,9 +24520,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J17" cm="1">
+      <c r="J17" t="str" cm="1">
         <f t="array" aca="1" ref="J17" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -24558,9 +24560,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J18" cm="1">
+      <c r="J18" t="str" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -24598,9 +24600,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J19" cm="1">
+      <c r="J19" t="str" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -24638,9 +24640,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J20" cm="1">
+      <c r="J20" t="str" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -24678,9 +24680,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J21" cm="1">
+      <c r="J21" t="str" cm="1">
         <f t="array" aca="1" ref="J21" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -24718,9 +24720,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J22" cm="1">
+      <c r="J22" t="str" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -24758,9 +24760,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J23" cm="1">
+      <c r="J23" t="str" cm="1">
         <f t="array" aca="1" ref="J23" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -24798,9 +24800,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J24" cm="1">
+      <c r="J24" t="str" cm="1">
         <f t="array" aca="1" ref="J24" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>
@@ -24895,9 +24897,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J2" cm="1">
+      <c r="J2" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -24935,9 +24937,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J3" cm="1">
+      <c r="J3" t="str" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -24975,9 +24977,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J4" cm="1">
+      <c r="J4" t="str" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -25015,9 +25017,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J5" cm="1">
+      <c r="J5" t="str" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -25055,9 +25057,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J6" cm="1">
+      <c r="J6" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -25095,9 +25097,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J7" cm="1">
+      <c r="J7" t="str" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -25135,9 +25137,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J8" cm="1">
+      <c r="J8" t="str" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -25175,9 +25177,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J9" cm="1">
+      <c r="J9" t="str" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -25215,9 +25217,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J10" cm="1">
+      <c r="J10" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -25255,9 +25257,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J11" cm="1">
+      <c r="J11" t="str" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -25295,9 +25297,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J12" cm="1">
+      <c r="J12" t="str" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -25335,9 +25337,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J13" cm="1">
+      <c r="J13" t="str" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -25375,9 +25377,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J14" cm="1">
+      <c r="J14" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -25415,9 +25417,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J15" cm="1">
+      <c r="J15" t="str" cm="1">
         <f t="array" aca="1" ref="J15" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -25455,9 +25457,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J16" cm="1">
+      <c r="J16" t="str" cm="1">
         <f t="array" aca="1" ref="J16" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -25495,9 +25497,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J17" cm="1">
+      <c r="J17" t="str" cm="1">
         <f t="array" aca="1" ref="J17" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -25535,9 +25537,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J18" cm="1">
+      <c r="J18" t="str" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -25575,9 +25577,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J19" cm="1">
+      <c r="J19" t="str" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -25615,9 +25617,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J20" cm="1">
+      <c r="J20" t="str" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -25655,9 +25657,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J21" cm="1">
+      <c r="J21" t="str" cm="1">
         <f t="array" aca="1" ref="J21" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -25695,9 +25697,9 @@
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="J22" cm="1">
+      <c r="J22" t="str" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>1.7</v>
+        <v>0.0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
16 Captured Russian territory reduced log mechanic change
</commit_message>
<xml_diff>
--- a/data/cards.xlsx
+++ b/data/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shipcards\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC657CD-E64A-44FF-8CA6-D69363AD4F4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A583F5EB-E722-4C07-A501-752619F3B66C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="771" firstSheet="3" activeTab="7" xr2:uid="{F50BFA29-F894-47F8-8978-4D4DA77633D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="771" firstSheet="2" activeTab="4" xr2:uid="{F50BFA29-F894-47F8-8978-4D4DA77633D4}"/>
   </bookViews>
   <sheets>
     <sheet name="military_asset_final" sheetId="7" r:id="rId1"/>
@@ -752,9 +752,6 @@
     <t>Grants 2 logistics capacity to the USN player if controlled by their opponent.</t>
   </si>
   <si>
-    <t>Provides -1 logistics capacity if owned by a non-Russian player.</t>
-  </si>
-  <si>
     <t>The F/A-18 is one of the longest-tenured and most battle-proven multi-role carrier aircraft in the world.</t>
   </si>
   <si>
@@ -1047,6 +1044,9 @@
   </si>
   <si>
     <t>0.0.1</t>
+  </si>
+  <si>
+    <t>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1230,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19BA67ED-4F2F-41CA-87A3-6166B158FDCE}" type="CELLRANGE">
+                    <a:fld id="{1093AD3B-FDD9-4BD6-A452-775BB22ABFB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1264,7 +1264,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E2B0500-1483-48A2-9DB7-2D2D99917D39}" type="CELLRANGE">
+                    <a:fld id="{CD29DDC8-BF31-4746-A47F-CD18A8F3C693}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1298,7 +1298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E74652AB-D54D-41E7-806F-819658DEF1A0}" type="CELLRANGE">
+                    <a:fld id="{3E3AE0DE-3F83-4E10-B073-B16092CE3A78}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1338,7 +1338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39894B46-29A0-4FC2-A910-27540CFA4590}" type="CELLRANGE">
+                    <a:fld id="{1D7B0C5B-B585-4A2C-9BAA-1E1DF105EDB8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1377,7 +1377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83A3DE41-B9ED-43B0-AF1B-E41308D6D5B7}" type="CELLRANGE">
+                    <a:fld id="{616841F2-87B9-4DE8-97A0-12B2176801DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1410,7 +1410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F53F70E-912F-49E8-AED7-B1D1EA67BCA2}" type="CELLRANGE">
+                    <a:fld id="{C5A5FFC1-1346-487E-9CE6-FA68B31E7D84}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1444,7 +1444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9019098A-83AE-4542-B790-4355FA624914}" type="CELLRANGE">
+                    <a:fld id="{EF71FAF7-A53C-4A45-ACAB-0E2C9D5325B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1484,7 +1484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{616FC26D-5A7D-4B09-B80A-AE45A4B1BD76}" type="CELLRANGE">
+                    <a:fld id="{F07A231E-65D6-42BF-A556-25C99F463107}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1523,7 +1523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07F33445-D379-4262-A89F-CF041F6D3D08}" type="CELLRANGE">
+                    <a:fld id="{06DB3F7C-006F-4A6A-A2D3-21B08D11D3F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1556,7 +1556,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA4398A4-CCDA-4103-8ED9-0331E9D4A557}" type="CELLRANGE">
+                    <a:fld id="{B2F02FBC-FED1-485A-90F5-D9CA707A2DAD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1596,7 +1596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F8E7AF0-3961-4275-BCD6-C0D6C2B378E7}" type="CELLRANGE">
+                    <a:fld id="{116EE131-CD51-4858-B06B-C321A76605F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1650,7 +1650,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{9E34D7E7-A15C-4811-9CD2-230BAC99A0E3}" type="CELLRANGE">
+                    <a:fld id="{65744709-D634-44EF-9C7D-A2DD050F75C1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -1720,7 +1720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0AB681F-341E-4FFA-ADCB-29964A00581A}" type="CELLRANGE">
+                    <a:fld id="{06DE9679-59FB-4C01-8818-C135F45D61ED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1760,7 +1760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DBAFC33-3F8F-4579-B0E3-60E1ECA3B0BF}" type="CELLRANGE">
+                    <a:fld id="{25E55B13-35FB-4646-9D99-9C08677996B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1799,7 +1799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0FCAD41C-10FD-441B-B5B1-EB8FE1EC9E46}" type="CELLRANGE">
+                    <a:fld id="{F8FCB11A-6B3B-46D6-B695-C0E81F9AB87D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1832,7 +1832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67DE8F01-B11E-45C3-BC67-DFA7E805815B}" type="CELLRANGE">
+                    <a:fld id="{C62E0FB3-E000-4112-81D5-011B101154FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1872,7 +1872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD823903-9C45-42B9-AD32-D2E4ECC135EB}" type="CELLRANGE">
+                    <a:fld id="{A9BDC099-171F-4A86-B4AF-41E650C33461}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1926,7 +1926,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{E161E9DB-9B33-44F7-B8A4-C1FF4535152A}" type="CELLRANGE">
+                    <a:fld id="{29134F01-4405-47B8-85AC-96E6F36E82AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -2002,7 +2002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7903D458-807C-46A6-A6AB-2BFBBD70CCF1}" type="CELLRANGE">
+                    <a:fld id="{99387B77-0E75-4738-87E4-A039F5DEA55B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2041,7 +2041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8180A7E4-2060-4688-B47C-A3A48CF709EE}" type="CELLRANGE">
+                    <a:fld id="{49177D63-6E9C-4CC6-8C3D-C8366CDCC699}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2080,7 +2080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81CC247B-EB05-43F1-8C11-F61E30A93409}" type="CELLRANGE">
+                    <a:fld id="{2D643E21-9B2C-444B-A99B-92D452335287}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2119,7 +2119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AD1A498-FB87-498E-B3D3-336B3BB56FE1}" type="CELLRANGE">
+                    <a:fld id="{5AC72BE9-CBFA-4842-8BAA-9631A152F404}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2152,7 +2152,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5CE632A-64D5-4D8C-A9A1-BA101A9EEF7B}" type="CELLRANGE">
+                    <a:fld id="{1CCE9ACB-33F5-4119-B71F-F6FDCF6C2EF7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2192,7 +2192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BFE0FD21-7B8C-4EBB-ADB4-D9C88F859919}" type="CELLRANGE">
+                    <a:fld id="{64DDDA78-AF72-49C1-B9FC-DEF5BF400EEF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2225,7 +2225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11D789D7-720A-48DA-901D-136427CE4D93}" type="CELLRANGE">
+                    <a:fld id="{7AE71BE6-709F-4B4D-9F02-5DB0D2D50E69}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2265,7 +2265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AD3F2A5-1B94-4325-964F-94BDF7AAF084}" type="CELLRANGE">
+                    <a:fld id="{1AC7D9AE-E07E-4C84-AA41-828C818DDE74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2298,7 +2298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{298D96FA-95B3-4FFE-8FB8-8A5FF872DCB5}" type="CELLRANGE">
+                    <a:fld id="{0DFA2A5D-F1DD-46BD-9967-0FFB25CCE48D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4019,7 +4019,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -4224,7 +4224,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
@@ -4292,7 +4292,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
@@ -4360,7 +4360,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
@@ -4567,7 +4567,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
@@ -4636,7 +4636,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
@@ -4705,7 +4705,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
@@ -4774,7 +4774,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
@@ -4977,7 +4977,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
@@ -5245,7 +5245,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
@@ -5312,7 +5312,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
@@ -5379,7 +5379,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
@@ -5446,7 +5446,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D25" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
@@ -5513,7 +5513,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D26" t="str" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
@@ -5581,7 +5581,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D27" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
@@ -5649,7 +5649,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D28" t="str" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
@@ -5717,7 +5717,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D29" t="str" cm="1">
         <f t="array" aca="1" ref="D29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
@@ -5785,7 +5785,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D30" t="str" cm="1">
         <f t="array" aca="1" ref="D30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
@@ -5853,7 +5853,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D31" t="str" cm="1">
         <f t="array" aca="1" ref="D31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
@@ -5922,7 +5922,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D32" t="str" cm="1">
         <f t="array" aca="1" ref="D32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
@@ -5991,7 +5991,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D33" t="str" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
@@ -6060,7 +6060,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D34" t="str" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
@@ -6129,7 +6129,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D35" t="str" cm="1">
         <f t="array" aca="1" ref="D35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
@@ -6198,7 +6198,7 @@
         <v>14</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D36" t="str" cm="1">
         <f t="array" aca="1" ref="D36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
@@ -6267,7 +6267,7 @@
         <v>15</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D37" t="str" cm="1">
         <f t="array" aca="1" ref="D37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
@@ -6335,7 +6335,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D38" t="str" cm="1">
         <f t="array" aca="1" ref="D38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
@@ -6403,7 +6403,7 @@
         <v>15</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D39" t="str" cm="1">
         <f t="array" aca="1" ref="D39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
@@ -6471,7 +6471,7 @@
         <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D40" t="str" cm="1">
         <f t="array" aca="1" ref="D40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
@@ -6539,7 +6539,7 @@
         <v>15</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D41" t="str" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
@@ -6809,7 +6809,7 @@
         <v>17</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D45" t="str" cm="1">
         <f t="array" aca="1" ref="D45" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B45)</f>
@@ -7280,7 +7280,7 @@
         <v>19</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D52" t="str" cm="1">
         <f t="array" aca="1" ref="D52" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B52)</f>
@@ -7348,7 +7348,7 @@
         <v>19</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D53" t="str" cm="1">
         <f t="array" aca="1" ref="D53" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B53)</f>
@@ -7484,7 +7484,7 @@
         <v>19</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D55" t="str" cm="1">
         <f t="array" aca="1" ref="D55" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B55)</f>
@@ -7552,7 +7552,7 @@
         <v>28</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D56" t="str" cm="1">
         <f t="array" aca="1" ref="D56" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B56)</f>
@@ -7620,7 +7620,7 @@
         <v>28</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D57" t="str" cm="1">
         <f t="array" aca="1" ref="D57" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B57)</f>
@@ -7688,7 +7688,7 @@
         <v>28</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D58" t="str" cm="1">
         <f t="array" aca="1" ref="D58" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B58)</f>
@@ -7756,7 +7756,7 @@
         <v>28</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D59" t="str" cm="1">
         <f t="array" aca="1" ref="D59" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B59)</f>
@@ -7891,7 +7891,7 @@
         <v>20</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D61" t="str" cm="1">
         <f t="array" aca="1" ref="D61" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B61)</f>
@@ -8303,7 +8303,7 @@
         <v>23</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D67" t="str" cm="1">
         <f t="array" aca="1" ref="D67" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B67)</f>
@@ -8372,7 +8372,7 @@
         <v>23</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D68" t="str" cm="1">
         <f t="array" aca="1" ref="D68" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B68)</f>
@@ -8648,7 +8648,7 @@
         <v>27</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D72" t="str" cm="1">
         <f t="array" aca="1" ref="D72" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B72)</f>
@@ -8717,7 +8717,7 @@
         <v>27</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D73" t="str" cm="1">
         <f t="array" aca="1" ref="D73" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B73)</f>
@@ -8786,7 +8786,7 @@
         <v>27</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D74" t="str" cm="1">
         <f t="array" aca="1" ref="D74" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B74)</f>
@@ -8993,7 +8993,7 @@
         <v>26</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D77" t="str" cm="1">
         <f t="array" aca="1" ref="D77" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B77)</f>
@@ -9062,7 +9062,7 @@
         <v>26</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D78" t="str" cm="1">
         <f t="array" aca="1" ref="D78" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B78)</f>
@@ -9269,7 +9269,7 @@
         <v>24</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D81" t="str" cm="1">
         <f t="array" aca="1" ref="D81" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B81)</f>
@@ -9337,7 +9337,7 @@
         <v>24</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D82" t="str" cm="1">
         <f t="array" aca="1" ref="D82" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B82)</f>
@@ -9405,7 +9405,7 @@
         <v>24</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D83" t="str" cm="1">
         <f t="array" aca="1" ref="D83" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B83)</f>
@@ -9533,7 +9533,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E3" t="s">
         <v>206</v>
@@ -9559,7 +9559,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E4" t="s">
         <v>104</v>
@@ -9592,7 +9592,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" t="s">
         <v>105</v>
@@ -9618,7 +9618,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E7" t="s">
         <v>106</v>
@@ -9635,7 +9635,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -9644,7 +9644,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E8" t="s">
         <v>107</v>
@@ -9670,7 +9670,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E9" t="s">
         <v>168</v>
@@ -9696,7 +9696,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E10" t="s">
         <v>108</v>
@@ -9722,7 +9722,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E11" t="s">
         <v>109</v>
@@ -9772,7 +9772,7 @@
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -9781,7 +9781,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E14" t="s">
         <v>111</v>
@@ -9807,7 +9807,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E15" t="s">
         <v>112</v>
@@ -9851,7 +9851,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -9860,10 +9860,10 @@
         <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -9891,7 +9891,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -9929,7 +9929,7 @@
         <v>170</v>
       </c>
       <c r="E22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -9966,7 +9966,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E25" t="s">
         <v>115</v>
@@ -9983,7 +9983,7 @@
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
@@ -9992,10 +9992,10 @@
         <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -10009,7 +10009,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -10018,10 +10018,10 @@
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -10035,7 +10035,7 @@
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -10044,10 +10044,10 @@
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -10684,7 +10684,7 @@
       </c>
       <c r="G14" t="str" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H14" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
@@ -10728,7 +10728,7 @@
       </c>
       <c r="G15" t="str" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H15" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
@@ -10772,7 +10772,7 @@
       </c>
       <c r="G16" t="str" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H16" t="str" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
@@ -10816,7 +10816,7 @@
       </c>
       <c r="G17" t="str" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H17" t="str" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
@@ -10860,7 +10860,7 @@
       </c>
       <c r="G18" t="str" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H18" t="str" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
@@ -10904,7 +10904,7 @@
       </c>
       <c r="G19" t="str" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H19" t="str" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
@@ -10948,7 +10948,7 @@
       </c>
       <c r="G20" t="str" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H20" t="str" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
@@ -10992,7 +10992,7 @@
       </c>
       <c r="G21" t="str" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H21" t="str" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
@@ -11036,7 +11036,7 @@
       </c>
       <c r="G22" t="str" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H22" t="str" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
@@ -11080,7 +11080,7 @@
       </c>
       <c r="G23" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H23" t="str" cm="1">
         <f t="array" aca="1" ref="H23" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
@@ -11124,7 +11124,7 @@
       </c>
       <c r="G24" t="str" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H24" t="str" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
@@ -11152,7 +11152,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D25" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
@@ -11168,7 +11168,7 @@
       </c>
       <c r="G25" t="str" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H25" t="str" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
@@ -11800,6 +11800,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -11868,7 +11872,7 @@
       </c>
       <c r="G2" t="str" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H2" t="str" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
@@ -11912,7 +11916,7 @@
       </c>
       <c r="G3" t="str" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H3" t="str" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
@@ -11956,7 +11960,7 @@
       </c>
       <c r="G4" t="str" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H4" t="str" cm="1">
         <f t="array" aca="1" ref="H4" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -12000,7 +12004,7 @@
       </c>
       <c r="G5" t="str" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H5" t="str" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
@@ -12044,7 +12048,7 @@
       </c>
       <c r="G6" t="str" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H6" t="str" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B6)</f>
@@ -12088,7 +12092,7 @@
       </c>
       <c r="G7" t="str" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H7" t="str" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
@@ -12132,7 +12136,7 @@
       </c>
       <c r="G8" t="str" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H8" t="str" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
@@ -12176,7 +12180,7 @@
       </c>
       <c r="G9" t="str" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H9" t="str" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
@@ -12220,7 +12224,7 @@
       </c>
       <c r="G10" t="str" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H10" t="str" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
@@ -12264,7 +12268,7 @@
       </c>
       <c r="G11" t="str" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H11" t="str" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
@@ -12308,7 +12312,7 @@
       </c>
       <c r="G12" t="str" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H12" t="str" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
@@ -12336,7 +12340,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
@@ -12352,7 +12356,7 @@
       </c>
       <c r="G13" t="str" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="H13" t="str" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">INDIRECT("territories!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
@@ -12382,7 +12386,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12424,7 +12428,7 @@
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -12504,7 +12508,7 @@
         <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H4" t="str">
         <f>version!$A$1</f>
@@ -12513,7 +12517,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -12523,7 +12527,7 @@
       </c>
       <c r="D5" s="1" t="str">
         <f>effects!$A$32</f>
-        <v>Provides -1 logistics capacity if owned by a non-Russian player.</v>
+        <v>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -15042,7 +15046,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -15247,7 +15251,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B7)</f>
@@ -15315,7 +15319,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B8)</f>
@@ -15383,7 +15387,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B9)</f>
@@ -15590,7 +15594,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
@@ -15659,7 +15663,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
@@ -15728,7 +15732,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B14)</f>
@@ -15797,7 +15801,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
@@ -16000,7 +16004,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
@@ -16268,7 +16272,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
@@ -16335,7 +16339,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B23)</f>
@@ -16402,7 +16406,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
@@ -16469,7 +16473,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D25" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B25)</f>
@@ -16536,7 +16540,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D26" t="str" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B26)</f>
@@ -16604,7 +16608,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D27" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
@@ -16672,7 +16676,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D28" t="str" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
@@ -16740,7 +16744,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D29" t="str" cm="1">
         <f t="array" aca="1" ref="D29" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B29)</f>
@@ -16808,7 +16812,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D30" t="str" cm="1">
         <f t="array" aca="1" ref="D30" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B30)</f>
@@ -16876,7 +16880,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D31" t="str" cm="1">
         <f t="array" aca="1" ref="D31" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B31)</f>
@@ -16945,7 +16949,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D32" t="str" cm="1">
         <f t="array" aca="1" ref="D32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
@@ -17014,7 +17018,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D33" t="str" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
@@ -17083,7 +17087,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D34" t="str" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
@@ -17152,7 +17156,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D35" t="str" cm="1">
         <f t="array" aca="1" ref="D35" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B35)</f>
@@ -17221,7 +17225,7 @@
         <v>14</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D36" t="str" cm="1">
         <f t="array" aca="1" ref="D36" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B36)</f>
@@ -17290,7 +17294,7 @@
         <v>15</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D37" t="str" cm="1">
         <f t="array" aca="1" ref="D37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
@@ -17358,7 +17362,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D38" t="str" cm="1">
         <f t="array" aca="1" ref="D38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
@@ -17426,7 +17430,7 @@
         <v>15</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D39" t="str" cm="1">
         <f t="array" aca="1" ref="D39" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
@@ -17494,7 +17498,7 @@
         <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D40" t="str" cm="1">
         <f t="array" aca="1" ref="D40" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B40)</f>
@@ -17562,7 +17566,7 @@
         <v>15</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D41" t="str" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
@@ -18043,7 +18047,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
@@ -18514,7 +18518,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B12)</f>
@@ -18582,7 +18586,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B13)</f>
@@ -18718,7 +18722,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B15)</f>
@@ -18786,7 +18790,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
@@ -18854,7 +18858,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B17)</f>
@@ -18922,7 +18926,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
@@ -18990,7 +18994,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B19)</f>
@@ -19125,7 +19129,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B21)</f>
@@ -19537,7 +19541,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D27" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
@@ -19606,7 +19610,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D28" t="str" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
@@ -19882,7 +19886,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D32" t="str" cm="1">
         <f t="array" aca="1" ref="D32" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B32)</f>
@@ -19951,7 +19955,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D33" t="str" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
@@ -20020,7 +20024,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D34" t="str" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B34)</f>
@@ -20227,7 +20231,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D37" t="str" cm="1">
         <f t="array" aca="1" ref="D37" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B37)</f>
@@ -20296,7 +20300,7 @@
         <v>26</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D38" t="str" cm="1">
         <f t="array" aca="1" ref="D38" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B38)</f>
@@ -20503,7 +20507,7 @@
         <v>24</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D41" t="str" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
@@ -20571,7 +20575,7 @@
         <v>24</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D42" t="str" cm="1">
         <f t="array" aca="1" ref="D42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
@@ -20639,7 +20643,7 @@
         <v>24</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D43" t="str" cm="1">
         <f t="array" aca="1" ref="D43" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B43)</f>
@@ -21142,7 +21146,7 @@
         <v>86</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N11" t="str">
         <f>version!$A$1</f>
@@ -21180,7 +21184,7 @@
         <v>87</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N12" t="str">
         <f>version!$A$1</f>
@@ -21219,7 +21223,7 @@
         <v>88</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N13" t="str">
         <f>version!$A$1</f>
@@ -21296,7 +21300,7 @@
         <v>90</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N15" t="str">
         <f>version!$A$1</f>
@@ -21408,7 +21412,7 @@
         <v>93</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N18" t="str">
         <f>version!$A$1</f>
@@ -21522,7 +21526,7 @@
         <v>96</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N21" t="str">
         <f>version!$A$1</f>
@@ -21561,7 +21565,7 @@
         <v>97</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N22" t="str">
         <f>version!$A$1</f>
@@ -21570,7 +21574,7 @@
     </row>
     <row r="23" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -21600,7 +21604,7 @@
         <v>98</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N23" t="str">
         <f>version!$A$1</f>
@@ -21638,7 +21642,7 @@
         <v>99</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N24" t="str">
         <f>version!$A$1</f>
@@ -21685,7 +21689,7 @@
     </row>
     <row r="26" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -21763,7 +21767,7 @@
     </row>
     <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -21789,10 +21793,10 @@
 </v>
       </c>
       <c r="L28" t="s">
+        <v>308</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="N28" t="str">
         <f>version!$A$1</f>
@@ -21809,8 +21813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5424B9FA-5F3A-48BD-A332-49100C2F7779}">
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21905,7 +21909,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -21915,7 +21919,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -21975,7 +21979,7 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>227</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -22003,7 +22007,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -22396,7 +22400,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
@@ -22436,7 +22440,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
@@ -22636,7 +22640,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
@@ -22796,7 +22800,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
@@ -22876,7 +22880,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
@@ -22956,7 +22960,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
@@ -23076,7 +23080,7 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D27" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B27)</f>
@@ -23116,7 +23120,7 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D28" t="str" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B28)</f>
@@ -23316,7 +23320,7 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D33" t="str" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B33)</f>
@@ -23556,7 +23560,7 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D39" t="str" cm="1">
         <f t="array" aca="1" ref="D39" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B39)</f>
@@ -23636,7 +23640,7 @@
         <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D41" t="str" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B41)</f>
@@ -23716,7 +23720,7 @@
         <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D43" t="str" cm="1">
         <f t="array" aca="1" ref="D43" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B43)</f>
@@ -23796,7 +23800,7 @@
         <v>27</v>
       </c>
       <c r="C45" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D45" t="str" cm="1">
         <f t="array" aca="1" ref="D45" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B45)</f>
@@ -23837,7 +23841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED05A72-9DE0-4247-9F2F-531B551ED433}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -24213,7 +24217,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
@@ -24253,7 +24257,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B11)</f>
@@ -24453,7 +24457,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
@@ -24613,7 +24617,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
@@ -24693,7 +24697,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>
@@ -24773,7 +24777,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B24)</f>
@@ -24950,7 +24954,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -24990,7 +24994,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B5)</f>
@@ -25190,7 +25194,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B10)</f>
@@ -25430,7 +25434,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B16)</f>
@@ -25510,7 +25514,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B18)</f>
@@ -25590,7 +25594,7 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B20)</f>
@@ -25670,7 +25674,7 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT("actions!"&amp;CHAR(COLUMN()+93)&amp;$B22)</f>

</xml_diff>

<commit_message>
some progress towards 0.0.1
</commit_message>
<xml_diff>
--- a/data/cards.xlsx
+++ b/data/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shipcards\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A583F5EB-E722-4C07-A501-752619F3B66C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64EA232-15DE-4BBA-A73C-6A25FFEBDE70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="771" firstSheet="2" activeTab="4" xr2:uid="{F50BFA29-F894-47F8-8978-4D4DA77633D4}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="327">
   <si>
     <t>Title</t>
   </si>
@@ -1047,6 +1047,9 @@
   </si>
   <si>
     <t>Partisans: Provides -4 logistics capacity if controlled by a non-Russian player.</t>
+  </si>
+  <si>
+    <t>CAP: +2 Help Defense</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1233,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1093AD3B-FDD9-4BD6-A452-775BB22ABFB3}" type="CELLRANGE">
+                    <a:fld id="{B31A5756-E93A-4C81-BFD5-02EFBB990D26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1264,7 +1267,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD29DDC8-BF31-4746-A47F-CD18A8F3C693}" type="CELLRANGE">
+                    <a:fld id="{97959442-8521-4D21-8485-9B09266DF168}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1298,7 +1301,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E3AE0DE-3F83-4E10-B073-B16092CE3A78}" type="CELLRANGE">
+                    <a:fld id="{0925825C-B1E3-4683-8B94-B6DCF555097F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1338,7 +1341,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D7B0C5B-B585-4A2C-9BAA-1E1DF105EDB8}" type="CELLRANGE">
+                    <a:fld id="{B5323A2F-2E8D-482F-B786-89DE3B0B2DF3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1377,7 +1380,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{616841F2-87B9-4DE8-97A0-12B2176801DB}" type="CELLRANGE">
+                    <a:fld id="{4EBB023C-E623-4366-8F1E-3F4EEB87564C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1410,7 +1413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5A5FFC1-1346-487E-9CE6-FA68B31E7D84}" type="CELLRANGE">
+                    <a:fld id="{8C393150-269B-46C4-B70E-95CD5EB1C260}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1444,7 +1447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF71FAF7-A53C-4A45-ACAB-0E2C9D5325B6}" type="CELLRANGE">
+                    <a:fld id="{04BABB3C-99F7-4B7D-A38A-30D8561FAC67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1484,7 +1487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F07A231E-65D6-42BF-A556-25C99F463107}" type="CELLRANGE">
+                    <a:fld id="{9C97ADE2-AA07-45BE-BC5A-4CA27A2ABBD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1523,7 +1526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06DB3F7C-006F-4A6A-A2D3-21B08D11D3F1}" type="CELLRANGE">
+                    <a:fld id="{5DECAA4E-ACFF-4E22-9596-06698ED7A12E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1556,7 +1559,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2F02FBC-FED1-485A-90F5-D9CA707A2DAD}" type="CELLRANGE">
+                    <a:fld id="{FBEC42DA-9BE9-46F9-B36A-92F30C23CB8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1596,7 +1599,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{116EE131-CD51-4858-B06B-C321A76605F0}" type="CELLRANGE">
+                    <a:fld id="{B601B1EC-C426-4FEE-8B71-277CFE8330F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1650,7 +1653,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{65744709-D634-44EF-9C7D-A2DD050F75C1}" type="CELLRANGE">
+                    <a:fld id="{EE3A188D-FBB7-482E-8025-EC6BBE66FF8E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -1720,7 +1723,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06DE9679-59FB-4C01-8818-C135F45D61ED}" type="CELLRANGE">
+                    <a:fld id="{26740249-B408-4AF3-AA54-88AE3F303A65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1760,7 +1763,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25E55B13-35FB-4646-9D99-9C08677996B0}" type="CELLRANGE">
+                    <a:fld id="{3010890D-B353-434F-8C2B-7C33CB97CBA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1799,7 +1802,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8FCB11A-6B3B-46D6-B695-C0E81F9AB87D}" type="CELLRANGE">
+                    <a:fld id="{3364D886-84A1-46F6-A9D5-0701FEC0E439}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1827,12 +1830,18 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.6668872417006637E-2"/>
+                  <c:y val="2.1802935010482211E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C62E0FB3-E000-4112-81D5-011B101154FB}" type="CELLRANGE">
+                    <a:fld id="{8511936F-7CA6-42A8-B2D2-46DED9B26DE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1841,7 +1850,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="l"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1851,7 +1860,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1872,7 +1880,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9BDC099-171F-4A86-B4AF-41E650C33461}" type="CELLRANGE">
+                    <a:fld id="{76B539EB-E815-46C0-B902-CA14062F5293}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1926,7 +1934,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{29134F01-4405-47B8-85AC-96E6F36E82AE}" type="CELLRANGE">
+                    <a:fld id="{143E84F7-A0F0-42E8-85DC-FF6DA16C727E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -2002,7 +2010,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99387B77-0E75-4738-87E4-A039F5DEA55B}" type="CELLRANGE">
+                    <a:fld id="{11ADF897-4037-43C5-8C3C-9741DA33B633}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2041,7 +2049,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49177D63-6E9C-4CC6-8C3D-C8366CDCC699}" type="CELLRANGE">
+                    <a:fld id="{ADF1C6E5-0244-4C85-944D-2B9682759F7C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2080,7 +2088,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D643E21-9B2C-444B-A99B-92D452335287}" type="CELLRANGE">
+                    <a:fld id="{41BB1F0D-3AA2-4C2C-8B28-1E24F88C6C21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2119,7 +2127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AC72BE9-CBFA-4842-8BAA-9631A152F404}" type="CELLRANGE">
+                    <a:fld id="{7690D551-B01F-40F5-84C8-032380D66A1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2152,7 +2160,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CCE9ACB-33F5-4119-B71F-F6FDCF6C2EF7}" type="CELLRANGE">
+                    <a:fld id="{1FBB4D66-CFAB-434C-9EC4-B0710543858A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2192,7 +2200,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64DDDA78-AF72-49C1-B9FC-DEF5BF400EEF}" type="CELLRANGE">
+                    <a:fld id="{3431988C-4BF2-49A9-9C0F-C4158B96FE01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2225,7 +2233,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AE71BE6-709F-4B4D-9F02-5DB0D2D50E69}" type="CELLRANGE">
+                    <a:fld id="{AFE95769-257C-4526-95A7-521558C8B8C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2265,7 +2273,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1AC7D9AE-E07E-4C84-AA41-828C818DDE74}" type="CELLRANGE">
+                    <a:fld id="{79FA131F-9664-4D7B-B0BE-18C091B05399}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2298,7 +2306,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DFA2A5D-F1DD-46BD-9967-0FFB25CCE48D}" type="CELLRANGE">
+                    <a:fld id="{B02D02E2-C7F0-4125-B14A-590E6751A82F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2508,10 +2516,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>11.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.5</c:v>
@@ -2550,7 +2558,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>12.5</c:v>
@@ -3909,7 +3917,7 @@
       </c>
       <c r="J2" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K2" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
@@ -3927,7 +3935,8 @@
         <f t="array" aca="1" ref="N2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2C Hawkeye: All squadrons you control in a combat including this asset have +1 attack and  defense.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O2" t="str" cm="1">
         <f t="array" aca="1" ref="O2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
@@ -3978,7 +3987,7 @@
       </c>
       <c r="J3" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K3" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
@@ -3996,7 +4005,8 @@
         <f t="array" aca="1" ref="N3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2C Hawkeye: All squadrons you control in a combat including this asset have +1 attack and  defense.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O3" t="str" cm="1">
         <f t="array" aca="1" ref="O3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
@@ -4047,7 +4057,7 @@
       </c>
       <c r="J4" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K4" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -4065,7 +4075,8 @@
         <f t="array" aca="1" ref="N4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2C Hawkeye: All squadrons you control in a combat including this asset have +1 attack and  defense.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O4" t="str" cm="1">
         <f t="array" aca="1" ref="O4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -6635,7 +6646,7 @@
       </c>
       <c r="J42" cm="1">
         <f t="array" aca="1" ref="J42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K42" cm="1">
         <f t="array" aca="1" ref="K42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
@@ -6652,7 +6663,8 @@
       <c r="N42" t="str" cm="1">
         <f t="array" aca="1" ref="N42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
         <v>STOBAR: Compatible with STOBAR and VTOL squadrons.
-Carrier 1: Can station 1 aircraft squadron.</v>
+Carrier 1: Can station 1 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O42" t="str" cm="1">
         <f t="array" aca="1" ref="O42" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B42)</f>
@@ -12559,8 +12571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8A294D-8A6F-470F-8FC6-DE99DB04E18C}">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="R77" sqref="R77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12648,7 +12660,7 @@
       </c>
       <c r="F2">
         <f>military_assets!G2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f>military_assets!H2</f>
@@ -12659,12 +12671,12 @@
         <v>USN</v>
       </c>
       <c r="J2">
-        <f>T17+T7</f>
-        <v>7.5</v>
+        <f>T17+T7+T8</f>
+        <v>10.5</v>
       </c>
       <c r="K2">
         <f>J2/G2</f>
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:L25" si="0">C2/G2</f>
@@ -12672,7 +12684,7 @@
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M25" si="1">F2/G2</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N2">
         <f t="shared" ref="N2:N25" si="2">E2/G2</f>
@@ -12680,15 +12692,15 @@
       </c>
       <c r="O2">
         <f>M2+L2+N2+K2</f>
-        <v>1.9166666666666665</v>
+        <v>2.0833333333333335</v>
       </c>
       <c r="P2">
         <f>L2+M2</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="Q2">
         <f>C2+E2/2+F2+J2</f>
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -12710,7 +12722,7 @@
       </c>
       <c r="F3">
         <f>military_assets!G3</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <f>military_assets!H3</f>
@@ -12721,12 +12733,12 @@
         <v>USN</v>
       </c>
       <c r="J3">
-        <f>T17+T7+T12</f>
-        <v>8</v>
+        <f>T17+T7+T12+T8</f>
+        <v>11</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K25" si="3">J3/G3</f>
-        <v>1.1428571428571428</v>
+        <v>1.5714285714285714</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
@@ -12734,7 +12746,7 @@
       </c>
       <c r="M3">
         <f t="shared" si="1"/>
-        <v>0.5714285714285714</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="N3">
         <f t="shared" si="2"/>
@@ -12742,15 +12754,15 @@
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O25" si="4">M3+L3+N3+K3</f>
-        <v>1.7142857142857142</v>
+        <v>1.8571428571428572</v>
       </c>
       <c r="P3">
         <f>L3+M3</f>
-        <v>0.5714285714285714</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q25" si="5">C3+E3/2+F3+J3</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -13578,7 +13590,7 @@
       </c>
       <c r="F16">
         <f>military_assets!G16</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16">
         <f>military_assets!H16</f>
@@ -13589,12 +13601,12 @@
         <v>RUS</v>
       </c>
       <c r="J16">
-        <f>T19</f>
-        <v>3</v>
+        <f>T19+T8</f>
+        <v>6</v>
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
@@ -13602,7 +13614,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N16">
         <f t="shared" si="2"/>
@@ -13610,15 +13622,15 @@
       </c>
       <c r="O16">
         <f t="shared" si="4"/>
-        <v>2.1666666666666665</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="P16">
         <f t="shared" si="6"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S16" t="s">
         <v>193</v>
@@ -14405,7 +14417,7 @@
       </c>
       <c r="O32">
         <f t="shared" ref="O32:O58" si="8">Q2</f>
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="33" spans="14:15" x14ac:dyDescent="0.25">
@@ -14415,7 +14427,7 @@
       </c>
       <c r="O33">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="14:15" x14ac:dyDescent="0.25">
@@ -14545,7 +14557,7 @@
       </c>
       <c r="O46">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="14:15" x14ac:dyDescent="0.25">
@@ -14936,7 +14948,7 @@
       </c>
       <c r="J2" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K2" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
@@ -14954,7 +14966,8 @@
         <f t="array" aca="1" ref="N2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2C Hawkeye: All squadrons you control in a combat including this asset have +1 attack and  defense.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O2" t="str" cm="1">
         <f t="array" aca="1" ref="O2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
@@ -15005,7 +15018,7 @@
       </c>
       <c r="J3" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K3" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
@@ -15023,7 +15036,8 @@
         <f t="array" aca="1" ref="N3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2C Hawkeye: All squadrons you control in a combat including this asset have +1 attack and  defense.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O3" t="str" cm="1">
         <f t="array" aca="1" ref="O3" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B3)</f>
@@ -15074,7 +15088,7 @@
       </c>
       <c r="J4" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K4" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -15092,7 +15106,8 @@
         <f t="array" aca="1" ref="N4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2C Hawkeye: All squadrons you control in a combat including this asset have +1 attack and  defense.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O4" t="str" cm="1">
         <f t="array" aca="1" ref="O4" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B4)</f>
@@ -17873,7 +17888,7 @@
       </c>
       <c r="J2" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K2" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
@@ -17890,7 +17905,8 @@
       <c r="N2" t="str" cm="1">
         <f t="array" aca="1" ref="N2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
         <v>STOBAR: Compatible with STOBAR and VTOL squadrons.
-Carrier 1: Can station 1 aircraft squadron.</v>
+Carrier 1: Can station 1 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="O2" t="str" cm="1">
         <f t="array" aca="1" ref="O2" ca="1">INDIRECT("military_assets!"&amp;CHAR(COLUMN()+93)&amp;$B2)</f>
@@ -20714,7 +20730,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20787,7 +20803,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>6</v>
@@ -20799,10 +20815,11 @@
         <v>18</v>
       </c>
       <c r="K2" s="1" t="str">
-        <f>effects!$A3&amp;CHAR(10)&amp;effects!$A4&amp;CHAR(10)&amp;effects!$A$31</f>
+        <f>effects!$A3&amp;CHAR(10)&amp;effects!$A4&amp;CHAR(10)&amp;effects!$A$31&amp;CHAR(10)&amp;effects!$A$34</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2C Hawkeye: All squadrons you control in a combat including this asset have +1 attack and  defense.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="L2" t="s">
         <v>77</v>
@@ -20826,7 +20843,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>7</v>
@@ -20838,10 +20855,11 @@
         <v>18</v>
       </c>
       <c r="K3" s="1" t="str">
-        <f>effects!$A3&amp;CHAR(10)&amp;effects!$A25&amp;CHAR(10)&amp;effects!$A$31</f>
+        <f>effects!$A3&amp;CHAR(10)&amp;effects!$A25&amp;CHAR(10)&amp;effects!$A$31&amp;CHAR(10)&amp;effects!$A$34</f>
         <v>CATOBAR: Compatible with CATOBAR, VTOL, and  STOBAR squadrons.
 E-2D Hawkeye-I: All friendly air squadrons in combat with this asset have +1 attack and  defense. Enemy air squadrons lose Ambush.
-Carrier 3: Can station 3 aircraft squadron.</v>
+Carrier 3: Can station 3 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="L3" t="s">
         <v>78</v>
@@ -21318,7 +21336,7 @@
         <v>2</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H16">
         <v>6</v>
@@ -21330,9 +21348,10 @@
         <v>18</v>
       </c>
       <c r="K16" s="1" t="str">
-        <f>effects!$A23&amp;CHAR(10)&amp;effects!$A$29</f>
+        <f>effects!$A23&amp;CHAR(10)&amp;effects!$A$29&amp;CHAR(10)&amp;effects!$A$34</f>
         <v>STOBAR: Compatible with STOBAR and VTOL squadrons.
-Carrier 1: Can station 1 aircraft squadron.</v>
+Carrier 1: Can station 1 aircraft squadron.
+CAP: +2 Help Defense</v>
       </c>
       <c r="L16" t="s">
         <v>91</v>
@@ -21814,7 +21833,7 @@
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21988,7 +22007,9 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>